<commit_message>
Update 2 - 11/1/2024 - 11:33 AM - JB
Added missing modules
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CB47EC-C526-44E9-9E5A-3FA87079D81D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD513F-6260-4894-BEE2-EC0B439AC36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -41,8 +41,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="49">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -87,9 +109,6 @@
   </si>
   <si>
     <t>You have had an opportunity to decide on a project and start the general set-up for the project. The next step is to go through and identify all the tasks that need to be commpleted to have a finished product for the Final Project Presentation. The Fibonacci Sequence to assign importance of each task. Rate the tasks by the importance of when they need to be done as well as the importance to the completion of the project. Some tasks with a low priority may never be completed. Those can be saved for a later project. Come back to this list each day, mark tasks that have been completed as "Done" and repriotize the remaining tasks.</t>
-  </si>
-  <si>
-    <t>Prriority</t>
   </si>
   <si>
     <t>This page is the last Scrum Form due and is  to record your final thoughts on the process</t>
@@ -170,7 +189,28 @@
     <t>Scrum Reports are based on Stories. Create a good story about what you want your project to do when it is completed.Tasks are often assigned as stories, with the author telling what they want each new portion of the project to do when it is complete.</t>
   </si>
   <si>
-    <t xml:space="preserve">A good game of Mancala can be hard to find. So I've been working to create a version of Mancala with as many programming languages as I can (with this being language number 3, after Java and C++). </t>
+    <t>https://github.com/JonathanBurg/Mancala-MASM</t>
+  </si>
+  <si>
+    <t>GitHub Repository:</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>readWrite</t>
+  </si>
+  <si>
+    <t>controller</t>
+  </si>
+  <si>
+    <t>board</t>
+  </si>
+  <si>
+    <t>A good game of Mancala can be hard to find. So I've been working to create a version of Mancala with as many programming languages as I can (with this being language number 3, after Java and C++). The game will have 2 DW arrays to store the number of stones in the 6 pits for each side and two DW variables for the number of stones in the Mancalas on the ends of the board. There will be 5 modules: one controlling the stones, one for printing the board, one for managing user input, the main module, and a read-write module. The module for managing user input will act as the driver for the program. The game will be turn based, with the board flipping after each move so the pits for the active player are on the bottom and their Mancala on the right. During a turn the active player will input a number to pick a pit on their side. The selected pit will be cleared and for the number of stones in the selected pit, each successive pit will be incremented, excluding the other player's Mancala. If the final stone lands in the active player's Mancala, they will get another turn. If the final stone ends in an empty pit on the active players side, that last stone and all the stones in the pit on the opposite side will be moved to the active player's Mancala. The game will end when there are no more uncaptured stones on the active player's side, or when there are no more uncaptured stones. The winner will be the player with the most stones in their Mancala. For the interface, an external library may be used to provide coloring to prevent mix-ups between who's turn it is.</t>
+  </si>
+  <si>
+    <t>boardController</t>
   </si>
 </sst>
 </file>
@@ -313,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +379,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -685,26 +728,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="66.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -712,7 +755,7 @@
         <v>45596</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -721,209 +764,232 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="12"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="str">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="str">
         <f>"Jonathan Burgener"</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),$C$10,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
       <c r="C12" t="str">
-        <f t="shared" ref="C12:C14" si="0">IF(NOT(ISBLANK(B12)),$C$10,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <f>IF(NOT(ISBLANK(B12)),$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
       <c r="C13" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <f t="shared" ref="C13:C14" si="0">IF(NOT(ISBLANK(B13)),$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="10" t="s">
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="str">
+        <f>IF(NOT(ISBLANK(B15)),$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="10"/>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="D17" s="11"/>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C18" s="2">
         <f>$C$3</f>
         <v>45600</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1">
+      <c r="D20" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C21" s="9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B22" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C23" s="13"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C24" s="13"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" s="13"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" s="13"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C28" s="13"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C29" s="13"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C30" s="13"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C31" s="13"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C32" s="13"/>
+      <c r="C24" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C32" s="14"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="13"/>
+      <c r="C33" s="14"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="13"/>
+      <c r="C34" s="14"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="13"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="13"/>
+      <c r="C36" s="14"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="13"/>
+      <c r="C37" s="14"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="13"/>
+      <c r="C38" s="14"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="13"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="13"/>
-    </row>
-    <row r="41" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="14"/>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C43" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="C22:C41"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="C24:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -934,8 +1000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,28 +1013,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>Cover!C3</f>
         <v>45600</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1017,10 +1083,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1031,38 +1097,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1075,7 +1157,7 @@
         <v>45600</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -1088,92 +1170,92 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>Cover!B18</f>
+        <f>Cover!B20</f>
         <v>All</v>
       </c>
       <c r="C18" t="str">
-        <f>Cover!C18</f>
+        <f>Cover!C20</f>
         <v>Decide on Project</v>
       </c>
       <c r="D18" s="1">
-        <f>Cover!D18</f>
+        <f>Cover!D20</f>
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>Cover!B19</f>
+        <f>Cover!B21</f>
         <v>All</v>
       </c>
       <c r="C19" t="str">
-        <f>Cover!C19</f>
+        <f>Cover!C21</f>
         <v>Identify major parts of the project</v>
       </c>
       <c r="D19" s="1">
-        <f>Cover!D19</f>
+        <f>Cover!D21</f>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>Cover!B20</f>
+        <f>Cover!B22</f>
         <v>All</v>
       </c>
       <c r="C20" t="str">
-        <f>Cover!C20</f>
+        <f>Cover!C22</f>
         <v>Set up GitHub account and invite all participants including WayneWCook</v>
       </c>
       <c r="D20" s="1">
-        <f>Cover!D20</f>
+        <f>Cover!D22</f>
         <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(NOT(ISBLANK(C21)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(NOT(ISBLANK(C22)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(NOT(ISBLANK(C23)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(NOT(ISBLANK(C24)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(NOT(ISBLANK(C25)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(NOT(ISBLANK(C26)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(NOT(ISBLANK(C27)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1196,108 +1278,108 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1314,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1327,28 +1409,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'4 Nov'!C3</f>
         <v>45603</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1397,10 +1479,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="11"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1411,38 +1493,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1455,7 +1553,7 @@
         <v>45603</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -1482,7 +1580,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
@@ -1496,7 +1594,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="str">
@@ -1510,7 +1608,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -1524,7 +1622,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -1538,7 +1636,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -1548,7 +1646,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -1558,7 +1656,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -1568,7 +1666,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -1578,7 +1676,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -1588,7 +1686,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(C28="","",Cover!$C$10)</f>
+        <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C28" t="str">
@@ -1615,109 +1713,109 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1735,7 +1833,7 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:D21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1747,28 +1845,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'7 Nov'!C3</f>
         <v>45607</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -1817,10 +1915,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1831,38 +1929,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1875,7 +1989,7 @@
         <v>45607</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -1888,7 +2002,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$10)</f>
+        <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="str">
@@ -1902,7 +2016,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
@@ -1916,7 +2030,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="str">
@@ -1930,7 +2044,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -1944,7 +2058,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -1958,7 +2072,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -1972,7 +2086,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -1986,7 +2100,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -2000,7 +2114,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -2014,7 +2128,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -2028,7 +2142,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(C28="","",Cover!$C$10)</f>
+        <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C28" t="str">
@@ -2059,79 +2173,79 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2148,8 +2262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2BDEB0-840B-4C3F-B27A-28B18F4DD1A5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2161,28 +2275,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'11 Nov'!C3</f>
         <v>45610</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2231,10 +2345,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2245,38 +2359,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2289,7 +2419,7 @@
         <v>45610</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -2302,7 +2432,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$10)</f>
+        <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C18" t="str">
@@ -2316,7 +2446,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C19" t="str">
@@ -2330,7 +2460,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C20" t="str">
@@ -2344,7 +2474,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -2358,7 +2488,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -2372,7 +2502,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -2386,7 +2516,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -2400,7 +2530,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -2414,7 +2544,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -2428,7 +2558,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -2442,7 +2572,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2465,97 +2595,97 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
-        <f>IF(NOT(ISBLANK(C46)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2572,8 +2702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2585,28 +2715,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'14 Nov'!C3</f>
         <v>45621</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -2655,10 +2785,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2669,38 +2799,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2713,7 +2859,7 @@
         <v>45621</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -2726,7 +2872,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$10)</f>
+        <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C18" t="str">
@@ -2740,7 +2886,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C19" t="str">
@@ -2754,7 +2900,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C20" t="str">
@@ -2768,7 +2914,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -2782,7 +2928,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -2796,7 +2942,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -2810,7 +2956,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -2824,7 +2970,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -2838,7 +2984,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -2852,7 +2998,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -2866,7 +3012,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2884,90 +3030,90 @@
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2984,8 +3130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D18"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2997,28 +3143,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'25 Nov'!C3</f>
         <v>45624</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -3067,10 +3213,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3081,38 +3227,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3125,7 +3287,7 @@
         <v>45624</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -3138,7 +3300,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$10)</f>
+        <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C18" t="str">
@@ -3152,7 +3314,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C19" t="str">
@@ -3166,7 +3328,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C20" t="str">
@@ -3180,7 +3342,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -3194,7 +3356,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -3208,7 +3370,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -3222,7 +3384,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -3236,7 +3398,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -3250,7 +3412,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -3264,7 +3426,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -3278,7 +3440,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3296,162 +3458,162 @@
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
-        <f>IF(NOT(ISBLANK(C46)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="str">
-        <f>IF(NOT(ISBLANK(C47)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="str">
-        <f>IF(NOT(ISBLANK(C48)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
-        <f>IF(NOT(ISBLANK(C49)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
-        <f>IF(NOT(ISBLANK(C50)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
-        <f>IF(NOT(ISBLANK(C51)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
-        <f>IF(NOT(ISBLANK(C52)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
-        <f>IF(NOT(ISBLANK(C53)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="str">
-        <f>IF(NOT(ISBLANK(C54)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="str">
-        <f>IF(NOT(ISBLANK(C55)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="str">
-        <f>IF(NOT(ISBLANK(C56)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3468,8 +3630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900E9D3-DDF2-4E4F-9A72-19E680A0FB5E}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3481,28 +3643,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <f>'28 Nov'!C3</f>
         <v>45628</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
@@ -3551,10 +3713,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3565,38 +3727,54 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3609,7 +3787,7 @@
         <v>45628</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -3622,7 +3800,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$10)</f>
+        <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C18" t="str">
@@ -3636,7 +3814,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$10)</f>
+        <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C19" t="str">
@@ -3650,7 +3828,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$10)</f>
+        <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C20" t="str">
@@ -3664,7 +3842,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$10)</f>
+        <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C21" t="str">
@@ -3678,7 +3856,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$10)</f>
+        <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C22" t="str">
@@ -3692,7 +3870,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$10)</f>
+        <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C23" t="str">
@@ -3706,7 +3884,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$10)</f>
+        <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C24" t="str">
@@ -3720,7 +3898,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$10)</f>
+        <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C25" t="str">
@@ -3734,7 +3912,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$10)</f>
+        <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C26" t="str">
@@ -3748,7 +3926,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$10)</f>
+        <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
       </c>
       <c r="C27" t="str">
@@ -3762,7 +3940,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3780,16 +3958,16 @@
         <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31">
         <v>1</v>
@@ -3797,11 +3975,11 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3809,11 +3987,11 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -3821,11 +3999,11 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -3833,229 +4011,229 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
-        <f>IF(NOT(ISBLANK(C46)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="str">
-        <f>IF(NOT(ISBLANK(C47)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="str">
-        <f>IF(NOT(ISBLANK(C48)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
-        <f>IF(NOT(ISBLANK(C49)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
-        <f>IF(NOT(ISBLANK(C50)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
-        <f>IF(NOT(ISBLANK(C51)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
-        <f>IF(NOT(ISBLANK(C52)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
-        <f>IF(NOT(ISBLANK(C53)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="str">
-        <f>IF(NOT(ISBLANK(C54)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="str">
-        <f>IF(NOT(ISBLANK(C55)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="str">
-        <f>IF(NOT(ISBLANK(C56)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="str">
-        <f>IF(NOT(ISBLANK(C57)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C57)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="str">
-        <f>IF(NOT(ISBLANK(C58)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C58)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="str">
-        <f>IF(NOT(ISBLANK(C59)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C59)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" t="str">
-        <f>IF(NOT(ISBLANK(C60)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C60)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" t="str">
-        <f>IF(NOT(ISBLANK(C61)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C61)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="str">
-        <f>IF(NOT(ISBLANK(C62)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C62)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="str">
-        <f>IF(NOT(ISBLANK(C63)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C63)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="str">
-        <f>IF(NOT(ISBLANK(C64)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C64)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="str">
-        <f>IF(NOT(ISBLANK(C65)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C65)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="str">
-        <f>IF(NOT(ISBLANK(C66)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C66)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="str">
-        <f>IF(NOT(ISBLANK(C67)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C67)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="str">
-        <f>IF(NOT(ISBLANK(C68)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C68)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="str">
-        <f>IF(NOT(ISBLANK(C69)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C69)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="str">
-        <f>IF(NOT(ISBLANK(C70)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C70)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="str">
-        <f>IF(NOT(ISBLANK(C71)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C71)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="str">
-        <f>IF(NOT(ISBLANK(C72)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C72)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -4072,8 +4250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B6CC2-E414-4E52-936B-7C04C3571020}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4085,28 +4263,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="F1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -4117,19 +4295,19 @@
         <v>45631</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
+        <v>18</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4148,15 +4326,15 @@
         <f>Cover!C4</f>
         <v>Manaca</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4166,15 +4344,15 @@
         <f>Cover!C5</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -4184,41 +4362,41 @@
         <f>Cover!C6</f>
         <v>ASCII Mancala Game</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="C8" s="17"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4227,105 +4405,121 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <v>main</v>
+      </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v>boardController</v>
+      </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
+        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -4335,224 +4529,224 @@
         <f>C2</f>
         <v>45631</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
-        <f>IF(NOT(ISBLANK(C18)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C18)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
-        <f>IF(NOT(ISBLANK(C19)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C19)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>IF(NOT(ISBLANK(C20)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C20)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D20">
         <v>3</v>
       </c>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>IF(NOT(ISBLANK(C21)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>IF(NOT(ISBLANK(C22)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
+        <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>IF(NOT(ISBLANK(C23)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
+        <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>IF(NOT(ISBLANK(C24)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
+        <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>IF(NOT(ISBLANK(C25)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
+        <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>IF(NOT(ISBLANK(C26)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
+        <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>IF(NOT(ISBLANK(C27)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
+        <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="10"/>
-      <c r="L28" s="10"/>
-      <c r="M28" s="10"/>
-      <c r="N28" s="10"/>
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -4562,15 +4756,15 @@
         <f>C3</f>
         <v>45632</v>
       </c>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
@@ -4579,120 +4773,120 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="10"/>
-      <c r="G30" s="10"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="10"/>
-      <c r="M30" s="10"/>
-      <c r="N30" s="10"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
+        <v>22</v>
+      </c>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="10"/>
-      <c r="K32" s="10"/>
-      <c r="L32" s="10"/>
-      <c r="M32" s="10"/>
-      <c r="N32" s="10"/>
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="10"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$10,"")</f>
-        <v/>
-      </c>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$10,"")</f>
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Update 3 - 11/6/2024 - 8:18 AM - JB Adding controls and some stubs
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD513F-6260-4894-BEE2-EC0B439AC36D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DA77A6-C86C-459F-8B8C-FAB1F07E4B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="52">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -147,12 +147,6 @@
     <t>Priority</t>
   </si>
   <si>
-    <t>To Be Determined</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Identify major parts of the project</t>
   </si>
   <si>
@@ -211,6 +205,21 @@
   </si>
   <si>
     <t>boardController</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Create Stubs and write main method.</t>
+  </si>
+  <si>
+    <t>Create basic board</t>
+  </si>
+  <si>
+    <t>Removed</t>
+  </si>
+  <si>
+    <t>Get basic controls set up</t>
   </si>
 </sst>
 </file>
@@ -303,7 +312,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -348,12 +357,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="1">
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal style="medium">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -413,6 +431,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,8 +749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4BDE91-026E-42C1-9643-D39E9BFB7C68}">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -777,7 +796,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -785,15 +804,15 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -812,7 +831,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" t="str">
         <f>"Jonathan Burgener"</f>
@@ -821,38 +840,48 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" t="str">
-        <f t="shared" ref="C13:C14" si="0">IF(NOT(ISBLANK(B13)),$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" t="str">
-        <f t="shared" si="0"/>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f>""</f>
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <f>IF(NOT(OR(ISBLANK(B16),B16="",B16=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
     </row>
     <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -898,7 +927,7 @@
         <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -909,7 +938,7 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1">
         <v>3</v>
@@ -917,15 +946,15 @@
     </row>
     <row r="23" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
@@ -1000,13 +1029,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
@@ -1098,11 +1127,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">Cover!B11:B16</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1111,7 +1140,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1120,7 +1149,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1129,7 +1158,7 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1138,13 +1167,16 @@
         <v>boardController</v>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1160,7 +1192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1168,7 +1200,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>Cover!B20</f>
         <v>All</v>
@@ -1181,8 +1213,11 @@
         <f>Cover!D20</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>Cover!B21</f>
         <v>All</v>
@@ -1195,8 +1230,11 @@
         <f>Cover!D21</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>Cover!B22</f>
         <v>All</v>
@@ -1209,57 +1247,60 @@
         <f>Cover!D22</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1268,7 +1309,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1276,27 +1317,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>23</v>
       </c>
       <c r="C31" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="D32" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1305,10 +1346,10 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>51</v>
+      </c>
+      <c r="D33" s="1">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -1396,13 +1437,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
@@ -1494,11 +1535,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">'4 Nov'!B10:B15</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1507,7 +1548,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1516,7 +1557,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1525,22 +1566,28 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" t="str">
+      <c r="B14" s="21" t="str">
         <v>boardController</v>
       </c>
-      <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+      <c r="C14" s="21" t="str">
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="E14" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -1573,9 +1620,9 @@
         <f>IF(ISBLANK('4 Nov'!C31),"",'4 Nov'!C31)</f>
         <v>Break up project into modules (use UML diagrams)</v>
       </c>
-      <c r="D18" s="1" t="str">
+      <c r="D18" s="1">
         <f>IF(ISBLANK('4 Nov'!D31),"",'4 Nov'!D31)</f>
-        <v>?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -1585,11 +1632,11 @@
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('4 Nov'!C32),"",'4 Nov'!C32)</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Create Stubs and write main method.</v>
+      </c>
+      <c r="D19" s="1">
         <f>IF(ISBLANK('4 Nov'!D32),"",'4 Nov'!D32)</f>
-        <v>?</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -1599,11 +1646,11 @@
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK('4 Nov'!C33),"",'4 Nov'!C33)</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D20" s="1" t="str">
+        <v>Get basic controls set up</v>
+      </c>
+      <c r="D20" s="1">
         <f>IF(ISBLANK('4 Nov'!D33),"",'4 Nov'!D33)</f>
-        <v>?</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -1717,35 +1764,25 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>28</v>
+        <v>49</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D32" s="1"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-      <c r="C33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D33" s="1"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
@@ -1833,12 +1870,12 @@
   <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
@@ -1930,11 +1967,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B13">'7 Nov'!B10:B13</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1943,7 +1980,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1952,7 +1989,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -1961,22 +1998,27 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
-        <v>boardController</v>
+        <f>""</f>
+        <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <f>""</f>
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2007,39 +2049,39 @@
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('7 Nov'!C31),"",'7 Nov'!C31)</f>
-        <v>To Be Determined</v>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>Create basic board</v>
+      </c>
+      <c r="D18" s="1">
         <f>IF(ISBLANK('7 Nov'!D31),"",'7 Nov'!D31)</f>
-        <v>?</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v>Jonathan Burgener</v>
+        <v/>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('7 Nov'!C32),"",'7 Nov'!C32)</f>
-        <v>To Be Determined</v>
+        <v/>
       </c>
       <c r="D19" s="1" t="str">
         <f>IF(ISBLANK('7 Nov'!D32),"",'7 Nov'!D32)</f>
-        <v>?</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
-        <v>Jonathan Burgener</v>
+        <v/>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK('7 Nov'!C33),"",'7 Nov'!C33)</f>
-        <v>To Be Determined</v>
+        <v/>
       </c>
       <c r="D20" s="1" t="str">
         <f>IF(ISBLANK('7 Nov'!D33),"",'7 Nov'!D33)</f>
-        <v>?</v>
+        <v/>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -2263,12 +2305,12 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.6640625" customWidth="1"/>
@@ -2360,11 +2402,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">'11 Nov'!B10:B15</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2373,7 +2415,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2382,7 +2424,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2391,22 +2433,25 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
-        <v>boardController</v>
+        <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2703,7 +2748,438 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2">
+        <f>'14 Nov'!C3</f>
+        <v>45621</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2">
+        <f>C2+3</f>
+        <v>45624</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="str">
+        <f>Cover!C4</f>
+        <v>Manaca</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="str">
+        <f>Cover!C5</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Cover!C6</f>
+        <v>ASCII Mancala Game</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B8" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="str" cm="1">
+        <f t="array" ref="B10:B15">'14 Nov'!B10:B15</f>
+        <v>main</v>
+      </c>
+      <c r="C10" t="str">
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B11" t="str">
+        <v>readWrite</v>
+      </c>
+      <c r="C11" t="str">
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B12" t="str">
+        <v>controller</v>
+      </c>
+      <c r="C12" t="str">
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B13" t="str">
+        <v>board</v>
+      </c>
+      <c r="C13" t="str">
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
+        <v>Jonathan Burgener</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B14" t="str">
+        <v/>
+      </c>
+      <c r="C14" t="str">
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16" s="2">
+        <f>C2</f>
+        <v>45621</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f>IF(C18="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <f>IF(ISBLANK('14 Nov'!C31),"",'14 Nov'!C31)</f>
+        <v/>
+      </c>
+      <c r="D18" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f>IF(C19="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <f>IF(ISBLANK('14 Nov'!C32),"",'14 Nov'!C32)</f>
+        <v/>
+      </c>
+      <c r="D19" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D32),"",'14 Nov'!D32)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f>IF(C20="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <f>IF(ISBLANK('14 Nov'!C33),"",'14 Nov'!C33)</f>
+        <v/>
+      </c>
+      <c r="D20" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D33),"",'14 Nov'!D33)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f>IF(C21="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <f>IF(ISBLANK('14 Nov'!C34),"",'14 Nov'!C34)</f>
+        <v/>
+      </c>
+      <c r="D21" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D34),"",'14 Nov'!D34)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="str">
+        <f>IF(C22="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C22" t="str">
+        <f>IF(ISBLANK('14 Nov'!C35),"",'14 Nov'!C35)</f>
+        <v/>
+      </c>
+      <c r="D22" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D35),"",'14 Nov'!D35)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" t="str">
+        <f>IF(C23="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C23" t="str">
+        <f>IF(ISBLANK('14 Nov'!C36),"",'14 Nov'!C36)</f>
+        <v/>
+      </c>
+      <c r="D23" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D36),"",'14 Nov'!D36)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B24" t="str">
+        <f>IF(C24="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C24" t="str">
+        <f>IF(ISBLANK('14 Nov'!C37),"",'14 Nov'!C37)</f>
+        <v/>
+      </c>
+      <c r="D24" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D37),"",'14 Nov'!D37)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B25" t="str">
+        <f>IF(C25="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C25" t="str">
+        <f>IF(ISBLANK('14 Nov'!C38),"",'14 Nov'!C38)</f>
+        <v/>
+      </c>
+      <c r="D25" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D38),"",'14 Nov'!D38)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="str">
+        <f>IF(C26="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C26" t="str">
+        <f>IF(ISBLANK('14 Nov'!C39),"",'14 Nov'!C39)</f>
+        <v/>
+      </c>
+      <c r="D26" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D39),"",'14 Nov'!D39)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B27" t="str">
+        <f>IF(C27="","",Cover!$C$11)</f>
+        <v/>
+      </c>
+      <c r="C27" t="str">
+        <f>IF(ISBLANK('14 Nov'!C40),"",'14 Nov'!C40)</f>
+        <v/>
+      </c>
+      <c r="D27" s="1" t="str">
+        <f>IF(ISBLANK('14 Nov'!D40),"",'14 Nov'!D40)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B28" t="str">
+        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2">
+        <f>C3</f>
+        <v>45624</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="str">
+        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B32" t="str">
+        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" t="str">
+        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B34" t="str">
+        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B35" t="str">
+        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B36" t="str">
+        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B42" t="str">
+        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B43" t="str">
+        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B44" t="str">
+        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
+  <dimension ref="A1:N56"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2732,8 +3208,8 @@
         <v>19</v>
       </c>
       <c r="C2" s="2">
-        <f>'14 Nov'!C3</f>
-        <v>45621</v>
+        <f>'25 Nov'!C3</f>
+        <v>45624</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -2753,8 +3229,8 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <f>C2+3</f>
-        <v>45624</v>
+        <f>C2+4</f>
+        <v>45628</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -2800,11 +3276,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">'25 Nov'!B10:B15</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2813,7 +3289,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2822,7 +3298,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -2831,22 +3307,25 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
-        <v>boardController</v>
+        <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -2856,7 +3335,7 @@
       </c>
       <c r="C16" s="2">
         <f>C2</f>
-        <v>45621</v>
+        <v>45624</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>26</v>
@@ -2876,11 +3355,11 @@
         <v/>
       </c>
       <c r="C18" t="str">
-        <f>IF(ISBLANK('14 Nov'!C31),"",'14 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
+        <f>IF(ISBLANK('25 Nov'!C31),"",'25 Nov'!C31)</f>
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <f>IF(ISBLANK('25 Nov'!D31),"",'25 Nov'!D31)</f>
         <v/>
       </c>
     </row>
@@ -2890,11 +3369,11 @@
         <v/>
       </c>
       <c r="C19" t="str">
-        <f>IF(ISBLANK('14 Nov'!C32),"",'14 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D32),"",'14 Nov'!D32)</f>
+        <f>IF(ISBLANK('25 Nov'!C32),"",'25 Nov'!C32)</f>
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <f>IF(ISBLANK('25 Nov'!D32),"",'25 Nov'!D32)</f>
         <v/>
       </c>
     </row>
@@ -2904,11 +3383,11 @@
         <v/>
       </c>
       <c r="C20" t="str">
-        <f>IF(ISBLANK('14 Nov'!C33),"",'14 Nov'!C33)</f>
-        <v/>
-      </c>
-      <c r="D20" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D33),"",'14 Nov'!D33)</f>
+        <f>IF(ISBLANK('25 Nov'!C33),"",'25 Nov'!C33)</f>
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <f>IF(ISBLANK('25 Nov'!D33),"",'25 Nov'!D33)</f>
         <v/>
       </c>
     </row>
@@ -2918,11 +3397,11 @@
         <v/>
       </c>
       <c r="C21" t="str">
-        <f>IF(ISBLANK('14 Nov'!C34),"",'14 Nov'!C34)</f>
-        <v/>
-      </c>
-      <c r="D21" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D34),"",'14 Nov'!D34)</f>
+        <f>IF(ISBLANK('25 Nov'!C34),"",'25 Nov'!C34)</f>
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <f>IF(ISBLANK('25 Nov'!D34),"",'25 Nov'!D34)</f>
         <v/>
       </c>
     </row>
@@ -2932,11 +3411,11 @@
         <v/>
       </c>
       <c r="C22" t="str">
-        <f>IF(ISBLANK('14 Nov'!C35),"",'14 Nov'!C35)</f>
-        <v/>
-      </c>
-      <c r="D22" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D35),"",'14 Nov'!D35)</f>
+        <f>IF(ISBLANK('25 Nov'!C35),"",'25 Nov'!C35)</f>
+        <v/>
+      </c>
+      <c r="D22" t="str">
+        <f>IF(ISBLANK('25 Nov'!D35),"",'25 Nov'!D35)</f>
         <v/>
       </c>
     </row>
@@ -2946,11 +3425,11 @@
         <v/>
       </c>
       <c r="C23" t="str">
-        <f>IF(ISBLANK('14 Nov'!C36),"",'14 Nov'!C36)</f>
-        <v/>
-      </c>
-      <c r="D23" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D36),"",'14 Nov'!D36)</f>
+        <f>IF(ISBLANK('25 Nov'!C36),"",'25 Nov'!C36)</f>
+        <v/>
+      </c>
+      <c r="D23" t="str">
+        <f>IF(ISBLANK('25 Nov'!D36),"",'25 Nov'!D36)</f>
         <v/>
       </c>
     </row>
@@ -2960,11 +3439,11 @@
         <v/>
       </c>
       <c r="C24" t="str">
-        <f>IF(ISBLANK('14 Nov'!C37),"",'14 Nov'!C37)</f>
-        <v/>
-      </c>
-      <c r="D24" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D37),"",'14 Nov'!D37)</f>
+        <f>IF(ISBLANK('25 Nov'!C37),"",'25 Nov'!C37)</f>
+        <v/>
+      </c>
+      <c r="D24" t="str">
+        <f>IF(ISBLANK('25 Nov'!D37),"",'25 Nov'!D37)</f>
         <v/>
       </c>
     </row>
@@ -2974,11 +3453,11 @@
         <v/>
       </c>
       <c r="C25" t="str">
-        <f>IF(ISBLANK('14 Nov'!C38),"",'14 Nov'!C38)</f>
-        <v/>
-      </c>
-      <c r="D25" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D38),"",'14 Nov'!D38)</f>
+        <f>IF(ISBLANK('25 Nov'!C38),"",'25 Nov'!C38)</f>
+        <v/>
+      </c>
+      <c r="D25" t="str">
+        <f>IF(ISBLANK('25 Nov'!D38),"",'25 Nov'!D38)</f>
         <v/>
       </c>
     </row>
@@ -2988,11 +3467,11 @@
         <v/>
       </c>
       <c r="C26" t="str">
-        <f>IF(ISBLANK('14 Nov'!C39),"",'14 Nov'!C39)</f>
-        <v/>
-      </c>
-      <c r="D26" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D39),"",'14 Nov'!D39)</f>
+        <f>IF(ISBLANK('25 Nov'!C39),"",'25 Nov'!C39)</f>
+        <v/>
+      </c>
+      <c r="D26" t="str">
+        <f>IF(ISBLANK('25 Nov'!D39),"",'25 Nov'!D39)</f>
         <v/>
       </c>
     </row>
@@ -3002,11 +3481,11 @@
         <v/>
       </c>
       <c r="C27" t="str">
-        <f>IF(ISBLANK('14 Nov'!C40),"",'14 Nov'!C40)</f>
-        <v/>
-      </c>
-      <c r="D27" s="1" t="str">
-        <f>IF(ISBLANK('14 Nov'!D40),"",'14 Nov'!D40)</f>
+        <f>IF(ISBLANK('25 Nov'!C40),"",'25 Nov'!C40)</f>
+        <v/>
+      </c>
+      <c r="D27" t="str">
+        <f>IF(ISBLANK('25 Nov'!D40),"",'25 Nov'!D40)</f>
         <v/>
       </c>
     </row>
@@ -3022,7 +3501,7 @@
       </c>
       <c r="C29" s="2">
         <f>C3</f>
-        <v>45624</v>
+        <v>45628</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -3114,6 +3593,78 @@
     <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B45" t="str">
+        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B46" t="str">
+        <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B47" t="str">
+        <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B48" t="str">
+        <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B49" t="str">
+        <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B50" t="str">
+        <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B51" t="str">
+        <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B52" t="str">
+        <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B53" t="str">
+        <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B54" t="str">
+        <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B55" t="str">
+        <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B56" t="str">
+        <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3126,12 +3677,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
-  <dimension ref="A1:N56"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900E9D3-DDF2-4E4F-9A72-19E680A0FB5E}">
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3160,8 +3711,8 @@
         <v>19</v>
       </c>
       <c r="C2" s="2">
-        <f>'25 Nov'!C3</f>
-        <v>45624</v>
+        <f>'28 Nov'!C3</f>
+        <v>45628</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>18</v>
@@ -3181,8 +3732,8 @@
         <v>12</v>
       </c>
       <c r="C3" s="2">
-        <f>C2+4</f>
-        <v>45628</v>
+        <f>C2+3</f>
+        <v>45631</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -3228,11 +3779,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">'28 Nov'!B10:B15</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -3241,7 +3792,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -3250,7 +3801,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
@@ -3259,22 +3810,25 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
-        <v>boardController</v>
+        <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
@@ -3284,7 +3838,7 @@
       </c>
       <c r="C16" s="2">
         <f>C2</f>
-        <v>45624</v>
+        <v>45628</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>26</v>
@@ -3304,11 +3858,11 @@
         <v/>
       </c>
       <c r="C18" t="str">
-        <f>IF(ISBLANK('25 Nov'!C31),"",'25 Nov'!C31)</f>
+        <f>IF(ISBLANK('28 Nov'!C31),"",'28 Nov'!C31)</f>
         <v/>
       </c>
       <c r="D18" t="str">
-        <f>IF(ISBLANK('25 Nov'!D31),"",'25 Nov'!D31)</f>
+        <f>IF(ISBLANK('28 Nov'!D31),"",'28 Nov'!D31)</f>
         <v/>
       </c>
     </row>
@@ -3318,11 +3872,11 @@
         <v/>
       </c>
       <c r="C19" t="str">
-        <f>IF(ISBLANK('25 Nov'!C32),"",'25 Nov'!C32)</f>
+        <f>IF(ISBLANK('28 Nov'!C32),"",'28 Nov'!C32)</f>
         <v/>
       </c>
       <c r="D19" t="str">
-        <f>IF(ISBLANK('25 Nov'!D32),"",'25 Nov'!D32)</f>
+        <f>IF(ISBLANK('28 Nov'!D32),"",'28 Nov'!D32)</f>
         <v/>
       </c>
     </row>
@@ -3332,11 +3886,11 @@
         <v/>
       </c>
       <c r="C20" t="str">
-        <f>IF(ISBLANK('25 Nov'!C33),"",'25 Nov'!C33)</f>
+        <f>IF(ISBLANK('28 Nov'!C33),"",'28 Nov'!C33)</f>
         <v/>
       </c>
       <c r="D20" t="str">
-        <f>IF(ISBLANK('25 Nov'!D33),"",'25 Nov'!D33)</f>
+        <f>IF(ISBLANK('28 Nov'!D33),"",'28 Nov'!D33)</f>
         <v/>
       </c>
     </row>
@@ -3346,11 +3900,11 @@
         <v/>
       </c>
       <c r="C21" t="str">
-        <f>IF(ISBLANK('25 Nov'!C34),"",'25 Nov'!C34)</f>
+        <f>IF(ISBLANK('28 Nov'!C34),"",'28 Nov'!C34)</f>
         <v/>
       </c>
       <c r="D21" t="str">
-        <f>IF(ISBLANK('25 Nov'!D34),"",'25 Nov'!D34)</f>
+        <f>IF(ISBLANK('28 Nov'!D34),"",'28 Nov'!D34)</f>
         <v/>
       </c>
     </row>
@@ -3360,11 +3914,11 @@
         <v/>
       </c>
       <c r="C22" t="str">
-        <f>IF(ISBLANK('25 Nov'!C35),"",'25 Nov'!C35)</f>
+        <f>IF(ISBLANK('28 Nov'!C35),"",'28 Nov'!C35)</f>
         <v/>
       </c>
       <c r="D22" t="str">
-        <f>IF(ISBLANK('25 Nov'!D35),"",'25 Nov'!D35)</f>
+        <f>IF(ISBLANK('28 Nov'!D35),"",'28 Nov'!D35)</f>
         <v/>
       </c>
     </row>
@@ -3374,11 +3928,11 @@
         <v/>
       </c>
       <c r="C23" t="str">
-        <f>IF(ISBLANK('25 Nov'!C36),"",'25 Nov'!C36)</f>
+        <f>IF(ISBLANK('28 Nov'!C36),"",'28 Nov'!C36)</f>
         <v/>
       </c>
       <c r="D23" t="str">
-        <f>IF(ISBLANK('25 Nov'!D36),"",'25 Nov'!D36)</f>
+        <f>IF(ISBLANK('28 Nov'!D36),"",'28 Nov'!D36)</f>
         <v/>
       </c>
     </row>
@@ -3388,11 +3942,11 @@
         <v/>
       </c>
       <c r="C24" t="str">
-        <f>IF(ISBLANK('25 Nov'!C37),"",'25 Nov'!C37)</f>
+        <f>IF(ISBLANK('28 Nov'!C37),"",'28 Nov'!C37)</f>
         <v/>
       </c>
       <c r="D24" t="str">
-        <f>IF(ISBLANK('25 Nov'!D37),"",'25 Nov'!D37)</f>
+        <f>IF(ISBLANK('28 Nov'!D37),"",'28 Nov'!D37)</f>
         <v/>
       </c>
     </row>
@@ -3402,11 +3956,11 @@
         <v/>
       </c>
       <c r="C25" t="str">
-        <f>IF(ISBLANK('25 Nov'!C38),"",'25 Nov'!C38)</f>
+        <f>IF(ISBLANK('28 Nov'!C38),"",'28 Nov'!C38)</f>
         <v/>
       </c>
       <c r="D25" t="str">
-        <f>IF(ISBLANK('25 Nov'!D38),"",'25 Nov'!D38)</f>
+        <f>IF(ISBLANK('28 Nov'!D38),"",'28 Nov'!D38)</f>
         <v/>
       </c>
     </row>
@@ -3416,11 +3970,11 @@
         <v/>
       </c>
       <c r="C26" t="str">
-        <f>IF(ISBLANK('25 Nov'!C39),"",'25 Nov'!C39)</f>
+        <f>IF(ISBLANK('28 Nov'!C39),"",'28 Nov'!C39)</f>
         <v/>
       </c>
       <c r="D26" t="str">
-        <f>IF(ISBLANK('25 Nov'!D39),"",'25 Nov'!D39)</f>
+        <f>IF(ISBLANK('28 Nov'!D39),"",'28 Nov'!D39)</f>
         <v/>
       </c>
     </row>
@@ -3430,11 +3984,11 @@
         <v/>
       </c>
       <c r="C27" t="str">
-        <f>IF(ISBLANK('25 Nov'!C40),"",'25 Nov'!C40)</f>
+        <f>IF(ISBLANK('28 Nov'!C40),"",'28 Nov'!C40)</f>
         <v/>
       </c>
       <c r="D27" t="str">
-        <f>IF(ISBLANK('25 Nov'!D40),"",'25 Nov'!D40)</f>
+        <f>IF(ISBLANK('28 Nov'!D40),"",'28 Nov'!D40)</f>
         <v/>
       </c>
     </row>
@@ -3450,7 +4004,7 @@
       </c>
       <c r="C29" s="2">
         <f>C3</f>
-        <v>45628</v>
+        <v>45631</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -3464,522 +4018,22 @@
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v/>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C31" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B33" t="str">
-        <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="str">
-        <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="str">
-        <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="str">
-        <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="str">
-        <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B38" t="str">
-        <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B39" t="str">
-        <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B40" t="str">
-        <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B41" t="str">
-        <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B42" t="str">
-        <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B43" t="str">
-        <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B44" t="str">
-        <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B45" t="str">
-        <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B46" t="str">
-        <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B47" t="str">
-        <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B48" t="str">
-        <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B49" t="str">
-        <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B50" t="str">
-        <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B51" t="str">
-        <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B52" t="str">
-        <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B53" t="str">
-        <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B54" t="str">
-        <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B55" t="str">
-        <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B56" t="str">
-        <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B8:C8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900E9D3-DDF2-4E4F-9A72-19E680A0FB5E}">
-  <dimension ref="A1:N72"/>
-  <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="2">
-        <f>'28 Nov'!C3</f>
-        <v>45628</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="2">
-        <f>C2+3</f>
-        <v>45631</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="str">
-        <f>Cover!C4</f>
-        <v>Manaca</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="str">
-        <f>Cover!C5</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="str">
-        <f>Cover!C6</f>
-        <v>ASCII Mancala Game</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
-        <v>main</v>
-      </c>
-      <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B11" t="str">
-        <v>readWrite</v>
-      </c>
-      <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B12" t="str">
-        <v>controller</v>
-      </c>
-      <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B13" t="str">
-        <v>board</v>
-      </c>
-      <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" t="str">
-        <v>boardController</v>
-      </c>
-      <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="2">
-        <f>C2</f>
-        <v>45628</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18" t="str">
-        <f>IF(C18="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C18" t="str">
-        <f>IF(ISBLANK('28 Nov'!C31),"",'28 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" t="str">
-        <f>IF(ISBLANK('28 Nov'!D31),"",'28 Nov'!D31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" t="str">
-        <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C19" t="str">
-        <f>IF(ISBLANK('28 Nov'!C32),"",'28 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" t="str">
-        <f>IF(ISBLANK('28 Nov'!D32),"",'28 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" t="str">
-        <f>IF(C20="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C20" t="str">
-        <f>IF(ISBLANK('28 Nov'!C33),"",'28 Nov'!C33)</f>
-        <v/>
-      </c>
-      <c r="D20" t="str">
-        <f>IF(ISBLANK('28 Nov'!D33),"",'28 Nov'!D33)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="str">
-        <f>IF(C21="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C21" t="str">
-        <f>IF(ISBLANK('28 Nov'!C34),"",'28 Nov'!C34)</f>
-        <v/>
-      </c>
-      <c r="D21" t="str">
-        <f>IF(ISBLANK('28 Nov'!D34),"",'28 Nov'!D34)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="str">
-        <f>IF(C22="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C22" t="str">
-        <f>IF(ISBLANK('28 Nov'!C35),"",'28 Nov'!C35)</f>
-        <v/>
-      </c>
-      <c r="D22" t="str">
-        <f>IF(ISBLANK('28 Nov'!D35),"",'28 Nov'!D35)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="str">
-        <f>IF(C23="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C23" t="str">
-        <f>IF(ISBLANK('28 Nov'!C36),"",'28 Nov'!C36)</f>
-        <v/>
-      </c>
-      <c r="D23" t="str">
-        <f>IF(ISBLANK('28 Nov'!D36),"",'28 Nov'!D36)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B24" t="str">
-        <f>IF(C24="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C24" t="str">
-        <f>IF(ISBLANK('28 Nov'!C37),"",'28 Nov'!C37)</f>
-        <v/>
-      </c>
-      <c r="D24" t="str">
-        <f>IF(ISBLANK('28 Nov'!D37),"",'28 Nov'!D37)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B25" t="str">
-        <f>IF(C25="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C25" t="str">
-        <f>IF(ISBLANK('28 Nov'!C38),"",'28 Nov'!C38)</f>
-        <v/>
-      </c>
-      <c r="D25" t="str">
-        <f>IF(ISBLANK('28 Nov'!D38),"",'28 Nov'!D38)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B26" t="str">
-        <f>IF(C26="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C26" t="str">
-        <f>IF(ISBLANK('28 Nov'!C39),"",'28 Nov'!C39)</f>
-        <v/>
-      </c>
-      <c r="D26" t="str">
-        <f>IF(ISBLANK('28 Nov'!D39),"",'28 Nov'!D39)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B27" t="str">
-        <f>IF(C27="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C27" t="str">
-        <f>IF(ISBLANK('28 Nov'!C40),"",'28 Nov'!C40)</f>
-        <v/>
-      </c>
-      <c r="D27" t="str">
-        <f>IF(ISBLANK('28 Nov'!D40),"",'28 Nov'!D40)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B28" t="str">
-        <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2">
-        <f>C3</f>
-        <v>45631</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B31" t="str">
-        <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
-      </c>
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B32" t="str">
-        <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -3991,7 +4045,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D33">
         <v>3</v>
@@ -4003,7 +4057,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D34">
         <v>4</v>
@@ -4250,8 +4304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B6CC2-E414-4E52-936B-7C04C3571020}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4417,11 +4471,11 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
-        <f t="array" ref="B10:B14">Cover!B11:B15</f>
+        <f t="array" ref="B10:B15">'2 Dec'!B10:B15</f>
         <v>main</v>
       </c>
       <c r="C10" t="str">
-        <f>IF(NOT(ISBLANK(B10)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="F10" s="11"/>
@@ -4439,7 +4493,7 @@
         <v>readWrite</v>
       </c>
       <c r="C11" t="str">
-        <f>IF(NOT(ISBLANK(B11)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="F11" s="11"/>
@@ -4457,7 +4511,7 @@
         <v>controller</v>
       </c>
       <c r="C12" t="str">
-        <f>IF(NOT(ISBLANK(B12)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="F12" s="11"/>
@@ -4475,7 +4529,7 @@
         <v>board</v>
       </c>
       <c r="C13" t="str">
-        <f>IF(NOT(ISBLANK(B13)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
       <c r="F13" s="11"/>
@@ -4490,11 +4544,11 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
-        <v>boardController</v>
+        <v/>
       </c>
       <c r="C14" t="str">
-        <f>IF(NOT(ISBLANK(B14)),Cover!$C$11,"")</f>
-        <v>Jonathan Burgener</v>
+        <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
+        <v/>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="11"/>
@@ -4507,8 +4561,11 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" t="str">
+        <v/>
+      </c>
       <c r="C15" t="str">
-        <f>IF(NOT(ISBLANK(B15)),Cover!$C$11,"")</f>
+        <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="F15" s="11"/>
@@ -4565,7 +4622,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -4586,7 +4643,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -4607,7 +4664,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -4628,7 +4685,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D21">
         <v>4</v>
@@ -4785,7 +4842,7 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Update 5 - 11/6/2024 - 10:05 AM - JB
Got distracted by fixing the board
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0DA77A6-C86C-459F-8B8C-FAB1F07E4B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924B156-EAA9-4CBD-972B-4EB04EB9DF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -401,6 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -431,7 +432,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,10 +816,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="12"/>
+      <c r="C9" s="13"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -885,10 +885,10 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -953,66 +953,66 @@
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="14"/>
+      <c r="C25" s="15"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="14"/>
+      <c r="C26" s="15"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="14"/>
+      <c r="C27" s="15"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="14"/>
+      <c r="C28" s="15"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="14"/>
+      <c r="C29" s="15"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="14"/>
+      <c r="C30" s="15"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="14"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="14"/>
+      <c r="C32" s="15"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="14"/>
+      <c r="C33" s="15"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="14"/>
+      <c r="C34" s="15"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="14"/>
+      <c r="C35" s="15"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="14"/>
+      <c r="C36" s="15"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="14"/>
+      <c r="C37" s="15"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="14"/>
+      <c r="C38" s="15"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="14"/>
+      <c r="C39" s="15"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="14"/>
+      <c r="C40" s="15"/>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="14"/>
+      <c r="C41" s="15"/>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="14"/>
+      <c r="C42" s="15"/>
     </row>
     <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="15"/>
+      <c r="C43" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1042,11 +1042,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1112,10 +1112,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1437,8 +1437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1450,11 +1450,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1520,10 +1520,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="12"/>
+      <c r="C8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1571,10 +1571,10 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="str">
+      <c r="B14" s="11" t="str">
         <v>boardController</v>
       </c>
-      <c r="C14" s="21" t="str">
+      <c r="C14" s="11" t="str">
         <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
@@ -1882,11 +1882,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1952,10 +1952,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2317,11 +2317,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2387,10 +2387,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2760,11 +2760,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2830,10 +2830,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3191,11 +3191,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3261,10 +3261,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3694,11 +3694,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3764,10 +3764,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="18"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4317,28 +4317,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -4351,17 +4351,17 @@
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4380,15 +4380,15 @@
         <f>Cover!C4</f>
         <v>Manaca</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4398,15 +4398,15 @@
         <f>Cover!C5</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -4416,41 +4416,41 @@
         <f>Cover!C6</f>
         <v>ASCII Mancala Game</v>
       </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="C8" s="18"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4459,15 +4459,15 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
@@ -4478,15 +4478,15 @@
         <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
@@ -4496,15 +4496,15 @@
         <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
@@ -4514,15 +4514,15 @@
         <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
@@ -4532,15 +4532,15 @@
         <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
@@ -4550,15 +4550,15 @@
         <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
@@ -4568,15 +4568,15 @@
         <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -4586,15 +4586,15 @@
         <f>C2</f>
         <v>45631</v>
       </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
@@ -4606,15 +4606,15 @@
       <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
@@ -4627,15 +4627,15 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
@@ -4648,15 +4648,15 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
@@ -4669,15 +4669,15 @@
       <c r="D20">
         <v>3</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
@@ -4690,120 +4690,120 @@
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -4813,15 +4813,15 @@
         <f>C3</f>
         <v>45632</v>
       </c>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
@@ -4830,15 +4830,15 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -4847,75 +4847,75 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="12"/>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="str">

</xml_diff>

<commit_message>
Update 7 - 11/8/2024 - 2:45 PM - JB
Added board to program. The board does not change in any way currently but it is getting printed.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B924B156-EAA9-4CBD-972B-4EB04EB9DF84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DEF2A-F8B6-41E5-AAE0-E2468C20EE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="55">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -216,10 +216,19 @@
     <t>Create basic board</t>
   </si>
   <si>
-    <t>Removed</t>
-  </si>
-  <si>
     <t>Get basic controls set up</t>
+  </si>
+  <si>
+    <t>Research formatting the console output in MASM</t>
+  </si>
+  <si>
+    <t>Removed to combine boardController and board</t>
+  </si>
+  <si>
+    <t>Have a hard time figuring out what is needed before I complete each part of the program</t>
+  </si>
+  <si>
+    <t>Done. Ran into issues with Unicode, but got it figured out.</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
@@ -1346,7 +1355,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D33" s="1">
         <v>3</v>
@@ -1437,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1579,7 +1588,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="E14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
@@ -1603,7 +1612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>'4 Nov'!B31</f>
         <v>All</v>
@@ -1624,8 +1633,11 @@
         <f>IF(ISBLANK('4 Nov'!D31),"",'4 Nov'!D31)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1638,8 +1650,11 @@
         <f>IF(ISBLANK('4 Nov'!D32),"",'4 Nov'!D32)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1652,8 +1667,11 @@
         <f>IF(ISBLANK('4 Nov'!D33),"",'4 Nov'!D33)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -1667,7 +1685,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -1681,7 +1699,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -1691,7 +1709,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -1701,7 +1719,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -1711,7 +1729,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -1721,7 +1739,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -1731,7 +1749,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -1741,7 +1759,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1750,7 +1768,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1758,7 +1776,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1767,22 +1785,33 @@
         <v>49</v>
       </c>
       <c r="D31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-      <c r="D32" s="1"/>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-      <c r="D33" s="1"/>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C33" t="str">
+        <f>C18</f>
+        <v>Break up project into modules (use UML diagrams)</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
@@ -1869,8 +1898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2034,7 +2063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2042,7 +2071,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2053,38 +2082,41 @@
       </c>
       <c r="D18" s="1">
         <f>IF(ISBLANK('7 Nov'!D31),"",'7 Nov'!D31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('7 Nov'!C32),"",'7 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Research formatting the console output in MASM</v>
+      </c>
+      <c r="D19" s="1">
         <f>IF(ISBLANK('7 Nov'!D32),"",'7 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK('7 Nov'!C33),"",'7 Nov'!C33)</f>
-        <v/>
-      </c>
-      <c r="D20" s="1" t="str">
+        <v>Break up project into modules (use UML diagrams)</v>
+      </c>
+      <c r="D20" s="1">
         <f>IF(ISBLANK('7 Nov'!D33),"",'7 Nov'!D33)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2098,7 +2130,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2112,7 +2144,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2126,7 +2158,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2140,7 +2172,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2154,7 +2186,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2168,7 +2200,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2182,7 +2214,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -2196,7 +2228,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2205,7 +2237,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2213,13 +2245,13 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>

</xml_diff>

<commit_message>
Update 8 - 11/11/2024 - 11:00 AM - JB
Adding Irvine
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86DEF2A-F8B6-41E5-AAE0-E2468C20EE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A8852-2B19-41B6-8F37-DC46B0964E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="60">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -229,6 +229,21 @@
   </si>
   <si>
     <t>Done. Ran into issues with Unicode, but got it figured out.</t>
+  </si>
+  <si>
+    <t>Connect controls to board</t>
+  </si>
+  <si>
+    <t>Pretty up the board</t>
+  </si>
+  <si>
+    <t>Create win state</t>
+  </si>
+  <si>
+    <t>Set up edge case scenarios (capturing, extra move, etc.)</t>
+  </si>
+  <si>
+    <t>Just going to push to the end when I have everything figured out.</t>
   </si>
 </sst>
 </file>
@@ -762,20 +777,20 @@
       <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -783,7 +798,7 @@
         <v>45596</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -792,7 +807,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -800,7 +815,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -808,7 +823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -816,7 +831,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
@@ -824,13 +839,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -838,7 +853,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -847,7 +862,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -856,7 +871,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -865,7 +880,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -874,7 +889,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>46</v>
       </c>
@@ -883,7 +898,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>""</f>
         <v/>
@@ -893,14 +908,14 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -909,7 +924,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -920,7 +935,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -931,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -942,7 +957,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -953,12 +968,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
@@ -966,61 +981,61 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="15"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="15"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="15"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="15"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="15"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="16"/>
     </row>
   </sheetData>
@@ -1038,19 +1053,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DDC301-48E9-474C-9B8D-1FA90964021A}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1063,7 +1078,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1084,7 +1099,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1093,7 +1108,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1117,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1126,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1120,13 +1135,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1134,7 +1149,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">Cover!B11:B16</f>
         <v>main</v>
@@ -1144,7 +1159,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1153,7 +1168,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1162,7 +1177,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1171,7 +1186,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v>boardController</v>
       </c>
@@ -1180,7 +1195,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1189,7 +1204,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1209,7 +1224,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Cover!B20</f>
         <v>All</v>
@@ -1226,7 +1241,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Cover!B21</f>
         <v>All</v>
@@ -1243,7 +1258,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Cover!B22</f>
         <v>All</v>
@@ -1260,56 +1275,56 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1318,7 +1333,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1326,7 +1341,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>23</v>
       </c>
@@ -1337,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1349,7 +1364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1361,73 +1376,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1446,19 +1461,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50F7190-C596-42CC-8496-9A58A8133598}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1471,7 +1486,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1492,7 +1507,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1501,7 +1516,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1510,7 +1525,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1519,7 +1534,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1528,13 +1543,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1542,7 +1557,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'4 Nov'!B10:B15</f>
         <v>main</v>
@@ -1552,7 +1567,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1561,7 +1576,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1570,7 +1585,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="str">
         <v>boardController</v>
       </c>
@@ -1591,7 +1606,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1600,7 +1615,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1612,7 +1627,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1620,7 +1635,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'4 Nov'!B31</f>
         <v>All</v>
@@ -1637,7 +1652,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1654,7 +1669,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1671,7 +1686,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -1685,7 +1700,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -1699,7 +1714,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -1709,7 +1724,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -1719,7 +1734,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -1729,7 +1744,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -1739,7 +1754,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -1749,7 +1764,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -1759,7 +1774,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1768,7 +1783,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1776,7 +1791,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1788,7 +1803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1800,7 +1815,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1813,73 +1828,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1898,19 +1913,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1923,7 +1938,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1944,7 +1959,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1953,7 +1968,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1962,7 +1977,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1971,7 +1986,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1980,13 +1995,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1994,7 +2009,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B13">'7 Nov'!B10:B13</f>
         <v>main</v>
@@ -2004,7 +2019,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2013,7 +2028,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2022,7 +2037,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2031,7 +2046,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>""</f>
         <v/>
@@ -2041,7 +2056,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>""</f>
         <v/>
@@ -2051,7 +2066,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2063,7 +2078,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2071,7 +2086,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2088,7 +2103,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2102,7 +2117,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2115,8 +2130,11 @@
         <f>IF(ISBLANK('7 Nov'!D33),"",'7 Nov'!D33)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2130,7 +2148,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2144,7 +2162,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2158,7 +2176,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2172,7 +2190,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2186,7 +2204,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2200,7 +2218,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2214,7 +2232,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -2228,7 +2246,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2237,7 +2255,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2245,79 +2263,91 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
@@ -2337,18 +2367,18 @@
   <dimension ref="A1:N46"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2361,7 +2391,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2382,7 +2412,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2391,7 +2421,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2400,7 +2430,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2409,7 +2439,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2418,13 +2448,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2432,7 +2462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'11 Nov'!B10:B15</f>
         <v>main</v>
@@ -2442,7 +2472,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2451,7 +2481,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2460,7 +2490,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2469,7 +2499,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -2478,7 +2508,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -2487,7 +2517,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2499,7 +2529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2507,35 +2537,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('11 Nov'!C31),"",'11 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>Connect controls to board</v>
+      </c>
+      <c r="D18" s="1">
         <f>IF(ISBLANK('11 Nov'!D31),"",'11 Nov'!D31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('11 Nov'!C32),"",'11 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Create win state</v>
+      </c>
+      <c r="D19" s="1">
         <f>IF(ISBLANK('11 Nov'!D32),"",'11 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -2549,7 +2579,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2563,7 +2593,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2577,7 +2607,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2591,7 +2621,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2605,7 +2635,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2619,7 +2649,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2633,7 +2663,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2647,13 +2677,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2662,7 +2692,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2670,97 +2700,103 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C31" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
@@ -2779,19 +2815,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2840,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2825,7 +2861,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2834,7 +2870,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2843,7 +2879,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2852,7 +2888,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2861,13 +2897,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2875,7 +2911,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'14 Nov'!B10:B15</f>
         <v>main</v>
@@ -2885,7 +2921,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2894,7 +2930,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2903,7 +2939,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2912,7 +2948,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -2921,7 +2957,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -2930,7 +2966,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2942,7 +2978,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2950,21 +2986,21 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('14 Nov'!C31),"",'14 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" s="1" t="str">
+        <v>Set up edge case scenarios (capturing, extra move, etc.)</v>
+      </c>
+      <c r="D18" s="1">
         <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
@@ -2978,7 +3014,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -2992,7 +3028,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3006,7 +3042,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3020,7 +3056,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3034,7 +3070,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3048,7 +3084,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3062,7 +3098,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3076,7 +3112,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3090,13 +3126,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3105,7 +3141,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3113,85 +3149,98 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C31" t="s">
+        <v>56</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C32" t="str">
+        <f>'11 Nov'!C20</f>
+        <v>Break up project into modules (use UML diagrams)</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
@@ -3210,19 +3259,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3284,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3256,7 +3305,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3265,7 +3314,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3274,7 +3323,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3283,7 +3332,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3292,13 +3341,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3306,7 +3355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'25 Nov'!B10:B15</f>
         <v>main</v>
@@ -3316,7 +3365,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3325,7 +3374,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3334,7 +3383,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3343,7 +3392,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3352,7 +3401,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3361,7 +3410,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3373,7 +3422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3381,35 +3430,35 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('25 Nov'!C31),"",'25 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" t="str">
+        <v>Pretty up the board</v>
+      </c>
+      <c r="D18">
         <f>IF(ISBLANK('25 Nov'!D31),"",'25 Nov'!D31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('25 Nov'!C32),"",'25 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" t="str">
+        <v>Break up project into modules (use UML diagrams)</v>
+      </c>
+      <c r="D19">
         <f>IF(ISBLANK('25 Nov'!D32),"",'25 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -3423,7 +3472,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3437,7 +3486,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3451,7 +3500,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3465,7 +3514,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3479,7 +3528,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3493,7 +3542,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3507,7 +3556,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3521,13 +3570,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3536,7 +3585,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3544,157 +3593,157 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
@@ -3714,18 +3763,18 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3738,7 +3787,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3759,7 +3808,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3768,7 +3817,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3777,7 +3826,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3786,7 +3835,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3795,13 +3844,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3809,7 +3858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'28 Nov'!B10:B15</f>
         <v>main</v>
@@ -3819,7 +3868,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3828,7 +3877,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3837,7 +3886,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3846,7 +3895,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3855,7 +3904,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3864,7 +3913,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3876,7 +3925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3884,7 +3933,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
@@ -3898,7 +3947,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
@@ -3912,7 +3961,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -3926,7 +3975,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3940,7 +3989,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3954,7 +4003,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3968,7 +4017,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3982,7 +4031,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3996,7 +4045,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -4010,7 +4059,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -4024,13 +4073,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4039,7 +4088,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4047,7 +4096,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4059,7 +4108,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4071,7 +4120,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4083,7 +4132,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4095,229 +4144,229 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f>IF(NOT(ISBLANK(C57)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f>IF(NOT(ISBLANK(C58)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f>IF(NOT(ISBLANK(C59)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f>IF(NOT(ISBLANK(C60)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f>IF(NOT(ISBLANK(C61)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f>IF(NOT(ISBLANK(C62)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f>IF(NOT(ISBLANK(C63)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f>IF(NOT(ISBLANK(C64)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f>IF(NOT(ISBLANK(C65)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
         <f>IF(NOT(ISBLANK(C66)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
         <f>IF(NOT(ISBLANK(C67)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
         <f>IF(NOT(ISBLANK(C68)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
         <f>IF(NOT(ISBLANK(C69)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
         <f>IF(NOT(ISBLANK(C70)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
         <f>IF(NOT(ISBLANK(C71)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
         <f>IF(NOT(ISBLANK(C72)),Cover!$C$11,"")</f>
         <v/>
@@ -4340,15 +4389,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4372,7 +4421,7 @@
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4395,7 +4444,7 @@
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -4404,7 +4453,7 @@
         <v>45632</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -4422,7 +4471,7 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -4440,7 +4489,7 @@
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -4458,7 +4507,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -4469,7 +4518,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
@@ -4484,7 +4533,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4501,7 +4550,7 @@
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'2 Dec'!B10:B15</f>
         <v>main</v>
@@ -4520,7 +4569,7 @@
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -4538,7 +4587,7 @@
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -4556,7 +4605,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -4574,7 +4623,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -4592,7 +4641,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -4610,7 +4659,7 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -4628,7 +4677,7 @@
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -4648,7 +4697,7 @@
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(NOT(ISBLANK(C18)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4669,7 +4718,7 @@
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(NOT(ISBLANK(C19)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4690,7 +4739,7 @@
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(NOT(ISBLANK(C20)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4711,7 +4760,7 @@
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4732,7 +4781,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
@@ -4747,7 +4796,7 @@
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
@@ -4762,7 +4811,7 @@
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
@@ -4777,7 +4826,7 @@
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
@@ -4792,7 +4841,7 @@
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
@@ -4807,7 +4856,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
@@ -4822,7 +4871,7 @@
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
@@ -4837,7 +4886,7 @@
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4855,7 +4904,7 @@
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4872,7 +4921,7 @@
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -4889,7 +4938,7 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
@@ -4904,7 +4953,7 @@
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
@@ -4919,7 +4968,7 @@
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
@@ -4934,7 +4983,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
@@ -4949,31 +4998,31 @@
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>

</xml_diff>

<commit_message>
Update 9 - 10/13/2024 - 9:39 AM - JB
Experementing with Irvine. But for now, I am going back to the normal output for simplicity sakes.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14A8852-2B19-41B6-8F37-DC46B0964E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15134D1C-7CA5-4029-91C6-019A1099EE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="3" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="61">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Just going to push to the end when I have everything figured out.</t>
+  </si>
+  <si>
+    <t>Going with Irvine, which means rewriting as the readWrite file as it is wont work with Irvine.</t>
   </si>
 </sst>
 </file>
@@ -1913,8 +1916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,6 +2119,9 @@
         <f>IF(ISBLANK('7 Nov'!D32),"",'7 Nov'!D32)</f>
         <v>3</v>
       </c>
+      <c r="E19" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
@@ -2366,8 +2372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2BDEB0-840B-4C3F-B27A-28B18F4DD1A5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update 10 - 11/15/2024 - 11:47 AM - JB
Got distracted by C++ colored output. New control handling for the board are not fully working since the variables for the pits are set values and can't be changed. Working on fixing that.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15134D1C-7CA5-4029-91C6-019A1099EE0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25774DC-6ADF-4492-84B1-1B740F4B3097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="4" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="62">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>Going with Irvine, which means rewriting as the readWrite file as it is wont work with Irvine.</t>
+  </si>
+  <si>
+    <t>Not Finished</t>
   </si>
 </sst>
 </file>
@@ -780,20 +783,20 @@
       <selection activeCell="C12" sqref="C12:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -801,7 +804,7 @@
         <v>45596</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -810,7 +813,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -818,7 +821,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -826,7 +829,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -834,7 +837,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
@@ -842,13 +845,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="13"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -856,7 +859,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -865,7 +868,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -874,7 +877,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -883,7 +886,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -892,7 +895,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>46</v>
       </c>
@@ -901,7 +904,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="str">
         <f>""</f>
         <v/>
@@ -911,14 +914,14 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="12"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -927,7 +930,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -938,7 +941,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -949,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -960,7 +963,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -971,12 +974,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
@@ -984,61 +987,61 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" s="15"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C38" s="15"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C39" s="15"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C40" s="15"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C41" s="15"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C42" s="15"/>
     </row>
-    <row r="43" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C43" s="16"/>
     </row>
   </sheetData>
@@ -1060,15 +1063,15 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1102,7 +1105,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1120,7 +1123,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1129,7 +1132,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1138,13 +1141,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1152,7 +1155,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">Cover!B11:B16</f>
         <v>main</v>
@@ -1162,7 +1165,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1180,7 +1183,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1189,7 +1192,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v>boardController</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1207,7 +1210,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1227,7 +1230,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>Cover!B20</f>
         <v>All</v>
@@ -1244,7 +1247,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>Cover!B21</f>
         <v>All</v>
@@ -1261,7 +1264,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>Cover!B22</f>
         <v>All</v>
@@ -1278,56 +1281,56 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1336,7 +1339,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1344,7 +1347,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>23</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1367,7 +1370,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1379,73 +1382,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1468,15 +1471,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1489,7 +1492,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1513,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1519,7 +1522,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +1540,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1546,13 +1549,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1560,7 +1563,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'4 Nov'!B10:B15</f>
         <v>main</v>
@@ -1570,7 +1573,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1579,7 +1582,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1588,7 +1591,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1597,7 +1600,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" s="11" t="str">
         <v>boardController</v>
       </c>
@@ -1609,7 +1612,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1618,7 +1621,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1638,7 +1641,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>'4 Nov'!B31</f>
         <v>All</v>
@@ -1655,7 +1658,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1672,7 +1675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1689,7 +1692,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -1703,7 +1706,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -1717,7 +1720,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -1727,7 +1730,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -1737,7 +1740,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -1747,7 +1750,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -1757,7 +1760,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -1767,7 +1770,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -1777,7 +1780,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1786,7 +1789,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1794,7 +1797,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1806,7 +1809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1818,7 +1821,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1831,73 +1834,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1916,19 +1919,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -1941,7 +1944,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1962,7 +1965,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1971,7 +1974,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1980,7 +1983,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1989,7 +1992,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1998,13 +2001,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2012,7 +2015,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B13">'7 Nov'!B10:B13</f>
         <v>main</v>
@@ -2022,7 +2025,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2040,7 +2043,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2049,7 +2052,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <f>""</f>
         <v/>
@@ -2059,7 +2062,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <f>""</f>
         <v/>
@@ -2069,7 +2072,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2106,7 +2109,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2123,7 +2126,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2140,7 +2143,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2154,7 +2157,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2168,7 +2171,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2182,7 +2185,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2196,7 +2199,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2210,7 +2213,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2224,7 +2227,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2238,7 +2241,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -2252,7 +2255,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2261,7 +2264,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2269,7 +2272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2281,7 +2284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2293,67 +2296,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
@@ -2372,19 +2375,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2BDEB0-840B-4C3F-B27A-28B18F4DD1A5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2397,7 +2400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2418,7 +2421,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2427,7 +2430,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2436,7 +2439,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2445,7 +2448,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2454,13 +2457,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'11 Nov'!B10:B15</f>
         <v>main</v>
@@ -2478,7 +2481,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2487,7 +2490,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2505,7 +2508,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -2514,7 +2517,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -2523,7 +2526,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2535,7 +2538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2543,7 +2546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2557,7 +2560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2570,8 +2573,11 @@
         <f>IF(ISBLANK('11 Nov'!D32),"",'11 Nov'!D32)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -2585,7 +2591,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2599,7 +2605,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2613,7 +2619,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2627,7 +2633,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2641,7 +2647,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2655,7 +2661,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2669,7 +2675,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2683,13 +2689,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2698,7 +2704,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2706,7 +2712,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2715,94 +2721,101 @@
         <v>58</v>
       </c>
       <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C32" t="str">
+        <f>C19</f>
+        <v>Create win state</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
@@ -2825,15 +2838,15 @@
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2846,7 +2859,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2867,7 +2880,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2876,7 +2889,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2885,7 +2898,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2894,7 +2907,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2903,13 +2916,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2917,7 +2930,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'14 Nov'!B10:B15</f>
         <v>main</v>
@@ -2927,7 +2940,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2936,7 +2949,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2945,7 +2958,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2954,7 +2967,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -2963,7 +2976,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -2972,7 +2985,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2984,7 +2997,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2992,7 +3005,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3003,24 +3016,24 @@
       </c>
       <c r="D18" s="1">
         <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('14 Nov'!C32),"",'14 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" s="1" t="str">
+        <v>Create win state</v>
+      </c>
+      <c r="D19" s="1">
         <f>IF(ISBLANK('14 Nov'!D32),"",'14 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -3034,7 +3047,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3048,7 +3061,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3062,7 +3075,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3076,7 +3089,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3090,7 +3103,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3104,7 +3117,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3118,7 +3131,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3132,13 +3145,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3147,7 +3160,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3155,7 +3168,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3167,7 +3180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3180,73 +3193,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
@@ -3269,15 +3282,15 @@
       <selection activeCell="B3" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3290,7 +3303,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3311,7 +3324,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3320,7 +3333,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3329,7 +3342,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3338,7 +3351,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3347,13 +3360,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3361,7 +3374,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'25 Nov'!B10:B15</f>
         <v>main</v>
@@ -3371,7 +3384,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3380,7 +3393,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3389,7 +3402,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3398,7 +3411,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3407,7 +3420,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3416,7 +3429,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3428,7 +3441,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3436,7 +3449,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3450,7 +3463,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3464,7 +3477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -3478,7 +3491,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3492,7 +3505,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3506,7 +3519,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3520,7 +3533,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3534,7 +3547,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3548,7 +3561,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3562,7 +3575,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3576,13 +3589,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3591,7 +3604,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3599,157 +3612,157 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
@@ -3772,15 +3785,15 @@
       <selection activeCell="B4" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -3793,7 +3806,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3814,7 +3827,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3823,7 +3836,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3832,7 +3845,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3841,7 +3854,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3850,13 +3863,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3864,7 +3877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'28 Nov'!B10:B15</f>
         <v>main</v>
@@ -3874,7 +3887,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3883,7 +3896,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3892,7 +3905,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3901,7 +3914,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3910,7 +3923,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3919,7 +3932,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3931,7 +3944,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3939,7 +3952,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v/>
@@ -3953,7 +3966,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v/>
@@ -3967,7 +3980,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -3981,7 +3994,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3995,7 +4008,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -4009,7 +4022,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -4023,7 +4036,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -4037,7 +4050,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -4051,7 +4064,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -4065,7 +4078,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -4079,13 +4092,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4094,7 +4107,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4102,7 +4115,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4114,7 +4127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4126,7 +4139,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4138,7 +4151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4150,229 +4163,229 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="str">
         <f>IF(NOT(ISBLANK(C57)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="str">
         <f>IF(NOT(ISBLANK(C58)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="str">
         <f>IF(NOT(ISBLANK(C59)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" t="str">
         <f>IF(NOT(ISBLANK(C60)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" t="str">
         <f>IF(NOT(ISBLANK(C61)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="str">
         <f>IF(NOT(ISBLANK(C62)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="str">
         <f>IF(NOT(ISBLANK(C63)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="str">
         <f>IF(NOT(ISBLANK(C64)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="str">
         <f>IF(NOT(ISBLANK(C65)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="str">
         <f>IF(NOT(ISBLANK(C66)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B67" t="str">
         <f>IF(NOT(ISBLANK(C67)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B68" t="str">
         <f>IF(NOT(ISBLANK(C68)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B69" t="str">
         <f>IF(NOT(ISBLANK(C69)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B70" t="str">
         <f>IF(NOT(ISBLANK(C70)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B71" t="str">
         <f>IF(NOT(ISBLANK(C71)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B72" t="str">
         <f>IF(NOT(ISBLANK(C72)),Cover!$C$11,"")</f>
         <v/>
@@ -4395,15 +4408,15 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -4427,7 +4440,7 @@
       <c r="M1" s="21"/>
       <c r="N1" s="21"/>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4450,7 +4463,7 @@
       <c r="M2" s="20"/>
       <c r="N2" s="20"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -4459,7 +4472,7 @@
         <v>45632</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -4477,7 +4490,7 @@
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -4495,7 +4508,7 @@
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -4513,7 +4526,7 @@
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -4524,7 +4537,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="18" t="s">
         <v>6</v>
       </c>
@@ -4539,7 +4552,7 @@
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4556,7 +4569,7 @@
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'2 Dec'!B10:B15</f>
         <v>main</v>
@@ -4575,7 +4588,7 @@
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -4593,7 +4606,7 @@
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -4611,7 +4624,7 @@
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -4629,7 +4642,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -4647,7 +4660,7 @@
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -4665,7 +4678,7 @@
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -4683,7 +4696,7 @@
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -4703,7 +4716,7 @@
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(NOT(ISBLANK(C18)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4724,7 +4737,7 @@
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(NOT(ISBLANK(C19)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4745,7 +4758,7 @@
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(NOT(ISBLANK(C20)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4766,7 +4779,7 @@
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4787,7 +4800,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
@@ -4802,7 +4815,7 @@
       <c r="M22" s="12"/>
       <c r="N22" s="12"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
@@ -4817,7 +4830,7 @@
       <c r="M23" s="12"/>
       <c r="N23" s="12"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
@@ -4832,7 +4845,7 @@
       <c r="M24" s="12"/>
       <c r="N24" s="12"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
@@ -4847,7 +4860,7 @@
       <c r="M25" s="12"/>
       <c r="N25" s="12"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
@@ -4862,7 +4875,7 @@
       <c r="M26" s="12"/>
       <c r="N26" s="12"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
@@ -4877,7 +4890,7 @@
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
@@ -4892,7 +4905,7 @@
       <c r="M28" s="12"/>
       <c r="N28" s="12"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4910,7 +4923,7 @@
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4927,7 +4940,7 @@
       <c r="M30" s="12"/>
       <c r="N30" s="12"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -4944,7 +4957,7 @@
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
@@ -4959,7 +4972,7 @@
       <c r="M32" s="12"/>
       <c r="N32" s="12"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
@@ -4974,7 +4987,7 @@
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
@@ -4989,7 +5002,7 @@
       <c r="M34" s="12"/>
       <c r="N34" s="12"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
@@ -5004,31 +5017,31 @@
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>

</xml_diff>

<commit_message>
Update 11 - 11/18/2024 - 11:48 AM - JB
Working on fixing board not updating
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25774DC-6ADF-4492-84B1-1B740F4B3097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB8F7F9-66B7-40DF-B576-3EA19A6FE102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="64">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -250,6 +250,12 @@
   </si>
   <si>
     <t>Not Finished</t>
+  </si>
+  <si>
+    <t>Somewhat finished, however terms are not updating for some reason.</t>
+  </si>
+  <si>
+    <t>Fix board not updating</t>
   </si>
 </sst>
 </file>
@@ -1919,7 +1925,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51155316-38BB-46D3-AE3F-BA55423B0250}">
   <dimension ref="A1:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -2375,8 +2381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C2BDEB0-840B-4C3F-B27A-28B18F4DD1A5}">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2559,6 +2565,9 @@
         <f>IF(ISBLANK('11 Nov'!D31),"",'11 Nov'!D31)</f>
         <v>1</v>
       </c>
+      <c r="E18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
@@ -2721,7 +2730,7 @@
         <v>58</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
@@ -2734,88 +2743,94 @@
         <v>Create win state</v>
       </c>
       <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C33" t="s">
+        <v>63</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
@@ -2834,7 +2849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -3016,7 +3031,7 @@
       </c>
       <c r="D18" s="1">
         <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -3030,21 +3045,21 @@
       </c>
       <c r="D19" s="1">
         <f>IF(ISBLANK('14 Nov'!D32),"",'14 Nov'!D32)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK('14 Nov'!C33),"",'14 Nov'!C33)</f>
-        <v/>
-      </c>
-      <c r="D20" s="1" t="str">
+        <v>Fix board not updating</v>
+      </c>
+      <c r="D20" s="1">
         <f>IF(ISBLANK('14 Nov'!D33),"",'14 Nov'!D33)</f>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update 12.5 - 11/18/2024 - 10:55 PM - JB
Forgot to update the SCRUM status
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB8F7F9-66B7-40DF-B576-3EA19A6FE102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D727858B-B8BE-48BA-A562-344670D76CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -256,6 +256,21 @@
   </si>
   <si>
     <t>Fix board not updating</t>
+  </si>
+  <si>
+    <t>Eh… Who needs a win state anyways.</t>
+  </si>
+  <si>
+    <t>Adjust output messages</t>
+  </si>
+  <si>
+    <t>DONE. Needs some output to explain weird changes to the board, but otherwise working as intended.</t>
+  </si>
+  <si>
+    <t>DONE. Everything was appearently working, I was just not using arrays correctly.</t>
+  </si>
+  <si>
+    <t>Finish win state</t>
   </si>
 </sst>
 </file>
@@ -265,7 +280,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +344,13 @@
       <b/>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -407,7 +429,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +490,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2849,8 +2872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3012,7 +3035,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3020,7 +3043,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3033,8 +3056,11 @@
         <f>IF(ISBLANK('14 Nov'!D31),"",'14 Nov'!D31)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3047,8 +3073,11 @@
         <f>IF(ISBLANK('14 Nov'!D32),"",'14 Nov'!D32)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3061,8 +3090,11 @@
         <f>IF(ISBLANK('14 Nov'!D33),"",'14 Nov'!D33)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3076,7 +3108,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3090,7 +3122,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3104,7 +3136,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3118,7 +3150,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3132,7 +3164,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3146,7 +3178,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3160,13 +3192,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3175,7 +3207,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3183,7 +3215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3195,7 +3227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3208,73 +3240,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B34" t="str">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C34" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="D34" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
@@ -3293,8 +3337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B3" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3495,29 +3539,29 @@
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C20" t="str">
         <f>IF(ISBLANK('25 Nov'!C33),"",'25 Nov'!C33)</f>
-        <v/>
-      </c>
-      <c r="D20" t="str">
+        <v>Adjust output messages</v>
+      </c>
+      <c r="D20">
         <f>IF(ISBLANK('25 Nov'!D33),"",'25 Nov'!D33)</f>
-        <v/>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="str">
+      <c r="B21" s="22" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
-        <v/>
-      </c>
-      <c r="C21" t="str">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C21" s="22" t="str">
         <f>IF(ISBLANK('25 Nov'!C34),"",'25 Nov'!C34)</f>
-        <v/>
-      </c>
-      <c r="D21" t="str">
+        <v>Finish win state</v>
+      </c>
+      <c r="D21" s="22">
         <f>IF(ISBLANK('25 Nov'!D34),"",'25 Nov'!D34)</f>
-        <v/>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update 13 - 11/20/2024 - 11:27 AM - JB
Working on converting to Irvine. Added procedure to clear the console, courtesy of AG (Don't know full name). Currently readWrite.asm is broken because Irvine changes are being tested in another program and will be added after it is working.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F93B783-3F6B-4080-959A-B8FD5A7EF171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF4A6B9-EE45-431C-8758-9992C3C4595D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
@@ -234,9 +234,6 @@
     <t>Connect controls to board</t>
   </si>
   <si>
-    <t>Pretty up the board</t>
-  </si>
-  <si>
     <t>Create win state</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Finish win state</t>
+  </si>
+  <si>
+    <t>Pretty up the board (Irvine)</t>
   </si>
 </sst>
 </file>
@@ -460,6 +460,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -490,7 +491,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,10 +875,10 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="13"/>
+      <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -944,10 +944,10 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="13"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1012,66 +1012,66 @@
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="15"/>
+      <c r="C25" s="16"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="15"/>
+      <c r="C26" s="16"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="15"/>
+      <c r="C27" s="16"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="15"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="15"/>
+      <c r="C29" s="16"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="15"/>
+      <c r="C30" s="16"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="15"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="15"/>
+      <c r="C32" s="16"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="15"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="15"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="15"/>
+      <c r="C35" s="16"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="15"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="15"/>
+      <c r="C37" s="16"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="15"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="15"/>
+      <c r="C39" s="16"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="15"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="15"/>
+      <c r="C41" s="16"/>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="15"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="16"/>
+      <c r="C43" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1101,11 +1101,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1171,10 +1171,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1509,11 +1509,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1579,10 +1579,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="13"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1961,11 +1961,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2031,10 +2031,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2152,7 +2152,7 @@
         <v>3</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -2169,7 +2169,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -2319,7 +2319,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D32">
         <v>2</v>
@@ -2417,11 +2417,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2487,10 +2487,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2589,7 +2589,7 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -2606,7 +2606,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -2750,7 +2750,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -2775,7 +2775,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33">
         <v>1</v>
@@ -2872,8 +2872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2885,11 +2885,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2955,10 +2955,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3057,7 +3057,7 @@
         <v>3</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
@@ -3074,7 +3074,7 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
@@ -3091,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
@@ -3221,7 +3221,7 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C31" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="D31">
         <v>2</v>
@@ -3246,21 +3246,21 @@
         <v>Jonathan Burgener</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D33">
         <v>3</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B34" s="22" t="str">
+      <c r="B34" s="12" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="C34" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D34" s="22">
+      <c r="C34" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="12">
         <v>4</v>
       </c>
     </row>
@@ -3338,7 +3338,7 @@
   <dimension ref="A1:N56"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3350,11 +3350,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3420,10 +3420,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('25 Nov'!C31),"",'25 Nov'!C31)</f>
-        <v>Pretty up the board</v>
+        <v>Pretty up the board (Irvine)</v>
       </c>
       <c r="D18">
         <f>IF(ISBLANK('25 Nov'!D31),"",'25 Nov'!D31)</f>
@@ -3551,15 +3551,15 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="22" t="str">
+      <c r="B21" s="12" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="C21" s="22" t="str">
+      <c r="C21" s="12" t="str">
         <f>IF(ISBLANK('25 Nov'!C34),"",'25 Nov'!C34)</f>
         <v>Finish win state</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="12">
         <f>IF(ISBLANK('25 Nov'!D34),"",'25 Nov'!D34)</f>
         <v>4</v>
       </c>
@@ -3853,11 +3853,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3923,10 +3923,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4476,28 +4476,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
       <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -4510,17 +4510,17 @@
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4539,15 +4539,15 @@
         <f>Cover!C4</f>
         <v>Manaca</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4557,15 +4557,15 @@
         <f>Cover!C5</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -4575,41 +4575,41 @@
         <f>Cover!C6</f>
         <v>ASCII Mancala Game</v>
       </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
+      <c r="C8" s="19"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4618,15 +4618,15 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
@@ -4637,15 +4637,15 @@
         <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
@@ -4655,15 +4655,15 @@
         <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
@@ -4673,15 +4673,15 @@
         <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
@@ -4691,15 +4691,15 @@
         <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
@@ -4709,15 +4709,15 @@
         <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
@@ -4727,15 +4727,15 @@
         <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -4745,15 +4745,15 @@
         <f>C2</f>
         <v>45631</v>
       </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
@@ -4765,15 +4765,15 @@
       <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
@@ -4786,15 +4786,15 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
@@ -4807,15 +4807,15 @@
       <c r="D19">
         <v>2</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
@@ -4828,15 +4828,15 @@
       <c r="D20">
         <v>3</v>
       </c>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
@@ -4849,120 +4849,120 @@
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
-      <c r="I25" s="12"/>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
-      <c r="I26" s="12"/>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="12"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -4972,15 +4972,15 @@
         <f>C3</f>
         <v>45632</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
@@ -4989,15 +4989,15 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -5006,75 +5006,75 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="12"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13"/>
+      <c r="M31" s="13"/>
+      <c r="N31" s="13"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+      <c r="L32" s="13"/>
+      <c r="M32" s="13"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+      <c r="L33" s="13"/>
+      <c r="M33" s="13"/>
+      <c r="N33" s="13"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="12"/>
-      <c r="K34" s="12"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+      <c r="L34" s="13"/>
+      <c r="M34" s="13"/>
+      <c r="N34" s="13"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="12"/>
-      <c r="J35" s="12"/>
-      <c r="K35" s="12"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+      <c r="L35" s="13"/>
+      <c r="M35" s="13"/>
+      <c r="N35" s="13"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="str">

</xml_diff>

<commit_message>
Update 14 - 11/23/2024 - 11:48 PM - JB
Went a little crazy with the changes. This update represents an entire day spent doing nothing but working on this project. Decided to be done with Irvine, it was way to much of a hasle. Finally added a win state. Split the driving process in controller.asm into multiple processes to make it easier to keep jumps straight. Decided to take the return address off of the stack for any process that loops back to start a new round and have the program end by calling a exitProgram in main.asm instead of going back through the recursive return addresses to get back to the start. Ran out of time to work on this for today, but the processes for capturing a pit are still a bit broken, and I was in the middle of adding a reference to board.asm from the postProcessing in controller.asm to get the correct pit that was captured. Need to add a new process in board.asm to get that number.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF4A6B9-EE45-431C-8758-9992C3C4595D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2773E-3699-4A21-BC83-5E44D461FA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t>Pretty up the board (Irvine)</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -2873,7 +2876,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3226,6 +3229,9 @@
       <c r="D31">
         <v>2</v>
       </c>
+      <c r="E31" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
@@ -3240,7 +3246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3251,8 +3257,11 @@
       <c r="D33">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="12" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3263,62 +3272,65 @@
       <c r="D34" s="12">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>

</xml_diff>

<commit_message>
Update 18 - 12/2/2024 - 12:26 PM - JB
Added color for placed stones
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F2773E-3699-4A21-BC83-5E44D461FA6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B280563-64AC-4618-A0AC-F8315AC91D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" activeTab="7" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="74">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -274,6 +274,18 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Finish tidying up the project</t>
+  </si>
+  <si>
+    <t>Add color for placed stones</t>
+  </si>
+  <si>
+    <t>Ughhh</t>
+  </si>
+  <si>
+    <t>Ran out of time</t>
   </si>
 </sst>
 </file>
@@ -283,7 +295,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +370,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -428,11 +448,12 @@
       </diagonal>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -494,8 +515,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="1" builtinId="15"/>
   </cellStyles>
@@ -812,7 +835,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -873,7 +896,7 @@
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="23" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1082,8 +1105,11 @@
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="C24:C43"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C7" r:id="rId1" xr:uid="{D04B4D29-E4BB-480C-8C62-68E6949D4818}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2875,7 +2901,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8735962-B793-4062-AE35-D28323021671}">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -3349,8 +3375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A620C275-88C7-4CD3-802A-FF3FD1CF6DED}">
   <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3512,7 +3538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3520,7 +3546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3533,8 +3559,11 @@
         <f>IF(ISBLANK('25 Nov'!D31),"",'25 Nov'!D31)</f>
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3547,8 +3576,11 @@
         <f>IF(ISBLANK('25 Nov'!D32),"",'25 Nov'!D32)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3561,8 +3593,11 @@
         <f>IF(ISBLANK('25 Nov'!D33),"",'25 Nov'!D33)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="12" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3575,8 +3610,11 @@
         <f>IF(ISBLANK('25 Nov'!D34),"",'25 Nov'!D34)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3590,7 +3628,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3604,7 +3642,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3618,7 +3656,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3632,7 +3670,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3646,7 +3684,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3660,13 +3698,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3675,7 +3713,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3683,16 +3721,28 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
-        <v/>
+        <v>Jonathan Burgener</v>
+      </c>
+      <c r="C32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
@@ -3852,8 +3902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900E9D3-DDF2-4E4F-9A72-19E680A0FB5E}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4015,7 +4065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -4023,35 +4073,41 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C18" t="str">
         <f>IF(ISBLANK('28 Nov'!C31),"",'28 Nov'!C31)</f>
-        <v/>
-      </c>
-      <c r="D18" t="str">
+        <v>Finish tidying up the project</v>
+      </c>
+      <c r="D18">
         <f>IF(ISBLANK('28 Nov'!D31),"",'28 Nov'!D31)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
-        <v/>
+        <v>Jonathan Burgener</v>
       </c>
       <c r="C19" t="str">
         <f>IF(ISBLANK('28 Nov'!C32),"",'28 Nov'!C32)</f>
-        <v/>
-      </c>
-      <c r="D19" t="str">
+        <v>Add color for placed stones</v>
+      </c>
+      <c r="D19">
         <f>IF(ISBLANK('28 Nov'!D32),"",'28 Nov'!D32)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -4065,7 +4121,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -4079,7 +4135,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -4093,7 +4149,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -4107,7 +4163,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -4121,7 +4177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -4135,7 +4191,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -4149,7 +4205,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -4163,13 +4219,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4178,7 +4234,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4186,7 +4242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4198,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4475,8 +4531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B6CC2-E414-4E52-936B-7C04C3571020}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4819,6 +4875,9 @@
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19" t="s">
+        <v>69</v>
+      </c>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
@@ -4839,6 +4898,9 @@
       </c>
       <c r="D20">
         <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>

</xml_diff>

<commit_message>
Update 19 - 12/2/2024 - 10:57 PM - JB
Ready for presentation, Added final bits of color I wanted.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B280563-64AC-4618-A0AC-F8315AC91D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2CD60B-7349-43B6-A9DD-F650587FA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" activeTab="7" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" activeTab="8" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -285,7 +285,7 @@
     <t>Ughhh</t>
   </si>
   <si>
-    <t>Ran out of time</t>
+    <t>Done, took longer than I wanted</t>
   </si>
 </sst>
 </file>
@@ -485,6 +485,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -515,7 +516,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -896,15 +896,15 @@
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="15"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -970,10 +970,10 @@
       </c>
     </row>
     <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
@@ -1038,66 +1038,66 @@
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C25" s="16"/>
+      <c r="C25" s="17"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C26" s="16"/>
+      <c r="C26" s="17"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C27" s="16"/>
+      <c r="C27" s="17"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C28" s="16"/>
+      <c r="C28" s="17"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C29" s="16"/>
+      <c r="C29" s="17"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C30" s="16"/>
+      <c r="C30" s="17"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C31" s="16"/>
+      <c r="C31" s="17"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C32" s="16"/>
+      <c r="C32" s="17"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" s="16"/>
+      <c r="C33" s="17"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" s="16"/>
+      <c r="C34" s="17"/>
     </row>
     <row r="35" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C35" s="16"/>
+      <c r="C35" s="17"/>
     </row>
     <row r="36" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C36" s="16"/>
+      <c r="C36" s="17"/>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C37" s="16"/>
+      <c r="C37" s="17"/>
     </row>
     <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" s="16"/>
+      <c r="C38" s="17"/>
     </row>
     <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" s="16"/>
+      <c r="C39" s="17"/>
     </row>
     <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" s="16"/>
+      <c r="C40" s="17"/>
     </row>
     <row r="41" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C41" s="16"/>
+      <c r="C41" s="17"/>
     </row>
     <row r="42" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C42" s="16"/>
+      <c r="C42" s="17"/>
     </row>
     <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C43" s="17"/>
+      <c r="C43" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1130,11 +1130,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1200,10 +1200,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1538,11 +1538,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -1608,10 +1608,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -1990,11 +1990,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2060,10 +2060,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2446,11 +2446,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2516,10 +2516,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -2914,11 +2914,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -2984,10 +2984,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3388,11 +3388,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3458,10 +3458,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -3902,8 +3902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4900E9D3-DDF2-4E4F-9A72-19E680A0FB5E}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3915,11 +3915,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
       <c r="D1" s="7" t="s">
         <v>26</v>
       </c>
@@ -3985,10 +3985,10 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4531,8 +4531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B6CC2-E414-4E52-936B-7C04C3571020}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4544,28 +4544,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="D1" s="6" t="s">
         <v>26</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
@@ -4578,17 +4578,17 @@
       <c r="E2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
@@ -4607,15 +4607,15 @@
         <f>Cover!C4</f>
         <v>Manaca</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
@@ -4625,15 +4625,15 @@
         <f>Cover!C5</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
@@ -4643,41 +4643,41 @@
         <f>Cover!C6</f>
         <v>ASCII Mancala Game</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="14"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
+      <c r="C8" s="20"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -4686,15 +4686,15 @@
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" t="str" cm="1">
@@ -4705,15 +4705,15 @@
         <f>IF(NOT(OR(ISBLANK(B10),B10="",B10=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
@@ -4723,15 +4723,15 @@
         <f>IF(NOT(OR(ISBLANK(B11),B11="",B11=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
@@ -4741,15 +4741,15 @@
         <f>IF(NOT(OR(ISBLANK(B12),B12="",B12=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B13" t="str">
@@ -4759,15 +4759,15 @@
         <f>IF(NOT(OR(ISBLANK(B13),B13="",B13=0)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
       </c>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B14" t="str">
@@ -4777,15 +4777,15 @@
         <f>IF(NOT(OR(ISBLANK(B14),B14="",B14=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B15" t="str">
@@ -4795,15 +4795,15 @@
         <f>IF(NOT(OR(ISBLANK(B15),B15="",B15=0)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+      <c r="N15" s="14"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -4813,15 +4813,15 @@
         <f>C2</f>
         <v>45631</v>
       </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B17" s="4" t="s">
@@ -4833,15 +4833,15 @@
       <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="14"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B18" t="str">
@@ -4854,15 +4854,15 @@
       <c r="D18">
         <v>1</v>
       </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+      <c r="N18" s="14"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B19" t="str">
@@ -4878,15 +4878,15 @@
       <c r="E19" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+      <c r="N19" s="14"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
@@ -4902,15 +4902,15 @@
       <c r="E20" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
@@ -4923,120 +4923,120 @@
       <c r="D21">
         <v>4</v>
       </c>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="14"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="14"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="13"/>
-      <c r="J23" s="13"/>
-      <c r="K23" s="13"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F24" s="13"/>
-      <c r="G24" s="13"/>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
-      <c r="J24" s="13"/>
-      <c r="K24" s="13"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="14"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
-      <c r="H25" s="13"/>
-      <c r="I25" s="13"/>
-      <c r="J25" s="13"/>
-      <c r="K25" s="13"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="14"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="14"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F28" s="13"/>
-      <c r="G28" s="13"/>
-      <c r="H28" s="13"/>
-      <c r="I28" s="13"/>
-      <c r="J28" s="13"/>
-      <c r="K28" s="13"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B29" s="4" t="s">
@@ -5046,15 +5046,15 @@
         <f>C3</f>
         <v>45632</v>
       </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
-      <c r="L29" s="13"/>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="14"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B30" s="4" t="s">
@@ -5063,15 +5063,15 @@
       <c r="C30" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13"/>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
@@ -5080,75 +5080,75 @@
       <c r="C31" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13"/>
-      <c r="H31" s="13"/>
-      <c r="I31" s="13"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="13"/>
-      <c r="L31" s="13"/>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F32" s="13"/>
-      <c r="G32" s="13"/>
-      <c r="H32" s="13"/>
-      <c r="I32" s="13"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="13"/>
-      <c r="H33" s="13"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="13"/>
-      <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F34" s="13"/>
-      <c r="G34" s="13"/>
-      <c r="H34" s="13"/>
-      <c r="I34" s="13"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="13"/>
-      <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="14"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
-      <c r="F35" s="13"/>
-      <c r="G35" s="13"/>
-      <c r="H35" s="13"/>
-      <c r="I35" s="13"/>
-      <c r="J35" s="13"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+      <c r="N35" s="14"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B36" t="str">

</xml_diff>

<commit_message>
Update 20 - 12/5/2024 - 7:41 PM - JB
Final update. Game completed. Could use some organization and optimization, but otherwise it is working wonderfully. Added presentation slide.
</commit_message>
<xml_diff>
--- a/Scrum Status Forms w Task List.xlsx
+++ b/Scrum Status Forms w Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\source\repos\MancalaASM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2CD60B-7349-43B6-A9DD-F650587FA276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB7C74E-482D-45A1-8AC5-A0E0DEB7DB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12240" activeTab="8" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="8" xr2:uid="{5969DE55-CD1B-4C6F-87B5-39DBF0EA983E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="74">
   <si>
     <t>Scrum Reporting Form</t>
   </si>
@@ -838,20 +838,20 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.88671875" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
@@ -859,7 +859,7 @@
         <v>45596</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -868,7 +868,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -876,7 +876,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
@@ -884,7 +884,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
@@ -892,7 +892,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>40</v>
       </c>
@@ -900,13 +900,13 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="15"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -914,7 +914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>41</v>
       </c>
@@ -923,7 +923,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>42</v>
       </c>
@@ -932,7 +932,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>43</v>
       </c>
@@ -941,7 +941,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>44</v>
       </c>
@@ -950,7 +950,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>46</v>
       </c>
@@ -959,7 +959,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f>""</f>
         <v/>
@@ -969,14 +969,14 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
@@ -985,7 +985,7 @@
         <v>45600</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
@@ -996,7 +996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>23</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>23</v>
       </c>
@@ -1029,12 +1029,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:5" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
         <v>28</v>
       </c>
@@ -1042,61 +1042,61 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C25" s="17"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C26" s="17"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C27" s="17"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C29" s="17"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C30" s="17"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C31" s="17"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C32" s="17"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="17"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="17"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="17"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="17"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="17"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="17"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="17"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="17"/>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="17"/>
     </row>
-    <row r="43" spans="3:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="18"/>
     </row>
   </sheetData>
@@ -1121,15 +1121,15 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1163,7 +1163,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1199,13 +1199,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">Cover!B11:B16</f>
         <v>main</v>
@@ -1223,7 +1223,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v>boardController</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1268,7 +1268,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1280,7 +1280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>Cover!B20</f>
         <v>All</v>
@@ -1305,7 +1305,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>Cover!B21</f>
         <v>All</v>
@@ -1322,7 +1322,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>Cover!B22</f>
         <v>All</v>
@@ -1339,56 +1339,56 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v/>
       </c>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>45603</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>23</v>
       </c>
@@ -1416,7 +1416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1428,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1440,73 +1440,73 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1529,15 +1529,15 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -1550,7 +1550,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -1571,7 +1571,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -1580,7 +1580,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -1607,13 +1607,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="15"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'4 Nov'!B10:B15</f>
         <v>main</v>
@@ -1631,7 +1631,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="str">
         <v>boardController</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -1679,7 +1679,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>'4 Nov'!B31</f>
         <v>All</v>
@@ -1716,7 +1716,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1733,7 +1733,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -1750,7 +1750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -1764,7 +1764,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -1778,7 +1778,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -1788,7 +1788,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -1798,7 +1798,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -1808,7 +1808,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -1818,7 +1818,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -1828,7 +1828,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -1838,7 +1838,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>45607</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1867,7 +1867,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1879,7 +1879,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -1892,73 +1892,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
@@ -1981,15 +1981,15 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2023,7 +2023,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2059,13 +2059,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B13">'7 Nov'!B10:B13</f>
         <v>main</v>
@@ -2083,7 +2083,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>""</f>
         <v/>
@@ -2120,7 +2120,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f>""</f>
         <v/>
@@ -2130,7 +2130,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2167,7 +2167,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2184,7 +2184,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2201,7 +2201,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2215,7 +2215,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2229,7 +2229,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2243,7 +2243,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2257,7 +2257,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2271,7 +2271,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2285,7 +2285,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2299,7 +2299,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(C28="","",Cover!$C$11)</f>
         <v/>
@@ -2313,7 +2313,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>45610</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2342,7 +2342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2354,67 +2354,67 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
@@ -2437,15 +2437,15 @@
       <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2479,7 +2479,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2488,7 +2488,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2515,13 +2515,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'11 Nov'!B10:B15</f>
         <v>main</v>
@@ -2539,7 +2539,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -2548,7 +2548,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -2557,7 +2557,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -2575,7 +2575,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -2584,7 +2584,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -2604,7 +2604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2621,7 +2621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -2638,7 +2638,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -2652,7 +2652,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -2666,7 +2666,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -2680,7 +2680,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -2694,7 +2694,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -2708,7 +2708,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -2722,7 +2722,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -2736,7 +2736,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -2750,13 +2750,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>45621</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2785,7 +2785,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2798,7 +2798,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -2810,79 +2810,79 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
@@ -2905,15 +2905,15 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -2947,7 +2947,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -2983,13 +2983,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2997,7 +2997,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'14 Nov'!B10:B15</f>
         <v>main</v>
@@ -3007,7 +3007,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3043,7 +3043,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3052,7 +3052,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3064,7 +3064,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3089,7 +3089,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3106,7 +3106,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3123,7 +3123,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -3137,7 +3137,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3151,7 +3151,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3165,7 +3165,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3179,7 +3179,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3193,7 +3193,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3207,7 +3207,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3221,13 +3221,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3236,7 +3236,7 @@
         <v>45624</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3244,7 +3244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3259,7 +3259,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3272,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3287,7 +3287,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3302,61 +3302,61 @@
         <v>69</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
@@ -3379,15 +3379,15 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3448,7 +3448,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3457,13 +3457,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'25 Nov'!B10:B15</f>
         <v>main</v>
@@ -3481,7 +3481,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -3517,7 +3517,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -3526,7 +3526,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3563,7 +3563,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3580,7 +3580,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3597,7 +3597,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="12" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -3614,7 +3614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -3628,7 +3628,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -3642,7 +3642,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -3656,7 +3656,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -3670,7 +3670,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -3684,7 +3684,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -3698,13 +3698,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>45628</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3733,7 +3733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -3745,145 +3745,145 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
@@ -3906,15 +3906,15 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>19</v>
       </c>
@@ -3948,7 +3948,7 @@
       <c r="M2" s="8"/>
       <c r="N2" s="8"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -3957,7 +3957,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -3966,7 +3966,7 @@
         <v>Manaca</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -3984,13 +3984,13 @@
         <v>ASCII Mancala Game</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="20"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'28 Nov'!B10:B15</f>
         <v>main</v>
@@ -4008,7 +4008,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -4017,7 +4017,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -4026,7 +4026,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -4035,7 +4035,7 @@
         <v>Jonathan Burgener</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -4044,7 +4044,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -4053,7 +4053,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -4065,7 +4065,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -4073,7 +4073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(C18="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -4090,7 +4090,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(C19="","",Cover!$C$11)</f>
         <v>Jonathan Burgener</v>
@@ -4107,7 +4107,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(C20="","",Cover!$C$11)</f>
         <v/>
@@ -4121,7 +4121,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(C21="","",Cover!$C$11)</f>
         <v/>
@@ -4135,7 +4135,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(C22="","",Cover!$C$11)</f>
         <v/>
@@ -4149,7 +4149,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(C23="","",Cover!$C$11)</f>
         <v/>
@@ -4163,7 +4163,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(C24="","",Cover!$C$11)</f>
         <v/>
@@ -4177,7 +4177,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(C25="","",Cover!$C$11)</f>
         <v/>
@@ -4191,7 +4191,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(C26="","",Cover!$C$11)</f>
         <v/>
@@ -4205,7 +4205,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(C27="","",Cover!$C$11)</f>
         <v/>
@@ -4219,13 +4219,13 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>45631</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -4242,7 +4242,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f>IF(NOT(ISBLANK(C31)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4254,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4266,7 +4266,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4278,7 +4278,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4290,229 +4290,229 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f>IF(NOT(ISBLANK(C41)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f>IF(NOT(ISBLANK(C42)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f>IF(NOT(ISBLANK(C43)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f>IF(NOT(ISBLANK(C44)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f>IF(NOT(ISBLANK(C45)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f>IF(NOT(ISBLANK(C46)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f>IF(NOT(ISBLANK(C47)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f>IF(NOT(ISBLANK(C48)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f>IF(NOT(ISBLANK(C49)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f>IF(NOT(ISBLANK(C50)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f>IF(NOT(ISBLANK(C51)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f>IF(NOT(ISBLANK(C52)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f>IF(NOT(ISBLANK(C53)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="str">
         <f>IF(NOT(ISBLANK(C54)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="str">
         <f>IF(NOT(ISBLANK(C55)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="str">
         <f>IF(NOT(ISBLANK(C56)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
         <f>IF(NOT(ISBLANK(C57)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
         <f>IF(NOT(ISBLANK(C58)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
         <f>IF(NOT(ISBLANK(C59)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
         <f>IF(NOT(ISBLANK(C60)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
         <f>IF(NOT(ISBLANK(C61)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
         <f>IF(NOT(ISBLANK(C62)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
         <f>IF(NOT(ISBLANK(C63)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="str">
         <f>IF(NOT(ISBLANK(C64)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="str">
         <f>IF(NOT(ISBLANK(C65)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="str">
         <f>IF(NOT(ISBLANK(C66)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" t="str">
         <f>IF(NOT(ISBLANK(C67)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
         <f>IF(NOT(ISBLANK(C68)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
         <f>IF(NOT(ISBLANK(C69)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
         <f>IF(NOT(ISBLANK(C70)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
         <f>IF(NOT(ISBLANK(C71)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
         <f>IF(NOT(ISBLANK(C72)),Cover!$C$11,"")</f>
         <v/>
@@ -4531,19 +4531,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184B6CC2-E414-4E52-936B-7C04C3571020}">
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -4567,7 +4567,7 @@
       <c r="M1" s="23"/>
       <c r="N1" s="23"/>
     </row>
-    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>1</v>
       </c>
@@ -4590,7 +4590,7 @@
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -4599,7 +4599,7 @@
         <v>45632</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -4617,7 +4617,7 @@
       <c r="M4" s="14"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -4635,7 +4635,7 @@
       <c r="M5" s="14"/>
       <c r="N5" s="14"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -4653,7 +4653,7 @@
       <c r="M6" s="14"/>
       <c r="N6" s="14"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -4664,7 +4664,7 @@
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
         <v>6</v>
       </c>
@@ -4679,7 +4679,7 @@
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -4696,7 +4696,7 @@
       <c r="M9" s="14"/>
       <c r="N9" s="14"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" t="str" cm="1">
         <f t="array" ref="B10:B15">'2 Dec'!B10:B15</f>
         <v>main</v>
@@ -4715,7 +4715,7 @@
       <c r="M10" s="14"/>
       <c r="N10" s="14"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <v>readWrite</v>
       </c>
@@ -4733,7 +4733,7 @@
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <v>controller</v>
       </c>
@@ -4751,7 +4751,7 @@
       <c r="M12" s="14"/>
       <c r="N12" s="14"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <v>board</v>
       </c>
@@ -4769,7 +4769,7 @@
       <c r="M13" s="14"/>
       <c r="N13" s="14"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <v/>
       </c>
@@ -4787,7 +4787,7 @@
       <c r="M14" s="14"/>
       <c r="N14" s="14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <v/>
       </c>
@@ -4805,7 +4805,7 @@
       <c r="M15" s="14"/>
       <c r="N15" s="14"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -4823,7 +4823,7 @@
       <c r="M16" s="14"/>
       <c r="N16" s="14"/>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>10</v>
       </c>
@@ -4843,7 +4843,7 @@
       <c r="M17" s="14"/>
       <c r="N17" s="14"/>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f>IF(NOT(ISBLANK(C18)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4864,7 +4864,7 @@
       <c r="M18" s="14"/>
       <c r="N18" s="14"/>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f>IF(NOT(ISBLANK(C19)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4888,7 +4888,7 @@
       <c r="M19" s="14"/>
       <c r="N19" s="14"/>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f>IF(NOT(ISBLANK(C20)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4912,7 +4912,7 @@
       <c r="M20" s="14"/>
       <c r="N20" s="14"/>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f>IF(NOT(ISBLANK(C21)),Cover!$C$11,"")</f>
         <v>Jonathan Burgener</v>
@@ -4922,6 +4922,9 @@
       </c>
       <c r="D21">
         <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -4933,7 +4936,7 @@
       <c r="M21" s="14"/>
       <c r="N21" s="14"/>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f>IF(NOT(ISBLANK(C22)),Cover!$C$11,"")</f>
         <v/>
@@ -4948,7 +4951,7 @@
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f>IF(NOT(ISBLANK(C23)),Cover!$C$11,"")</f>
         <v/>
@@ -4963,7 +4966,7 @@
       <c r="M23" s="14"/>
       <c r="N23" s="14"/>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f>IF(NOT(ISBLANK(C24)),Cover!$C$11,"")</f>
         <v/>
@@ -4978,7 +4981,7 @@
       <c r="M24" s="14"/>
       <c r="N24" s="14"/>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f>IF(NOT(ISBLANK(C25)),Cover!$C$11,"")</f>
         <v/>
@@ -4993,7 +4996,7 @@
       <c r="M25" s="14"/>
       <c r="N25" s="14"/>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f>IF(NOT(ISBLANK(C26)),Cover!$C$11,"")</f>
         <v/>
@@ -5008,7 +5011,7 @@
       <c r="M26" s="14"/>
       <c r="N26" s="14"/>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f>IF(NOT(ISBLANK(C27)),Cover!$C$11,"")</f>
         <v/>
@@ -5023,7 +5026,7 @@
       <c r="M27" s="14"/>
       <c r="N27" s="14"/>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f>IF(NOT(ISBLANK(C28)),Cover!$C$11,"")</f>
         <v/>
@@ -5038,7 +5041,7 @@
       <c r="M28" s="14"/>
       <c r="N28" s="14"/>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>9</v>
       </c>
@@ -5056,7 +5059,7 @@
       <c r="M29" s="14"/>
       <c r="N29" s="14"/>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>10</v>
       </c>
@@ -5073,7 +5076,7 @@
       <c r="M30" s="14"/>
       <c r="N30" s="14"/>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>37</v>
       </c>
@@ -5090,7 +5093,7 @@
       <c r="M31" s="14"/>
       <c r="N31" s="14"/>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f>IF(NOT(ISBLANK(C32)),Cover!$C$11,"")</f>
         <v/>
@@ -5105,7 +5108,7 @@
       <c r="M32" s="14"/>
       <c r="N32" s="14"/>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f>IF(NOT(ISBLANK(C33)),Cover!$C$11,"")</f>
         <v/>
@@ -5120,7 +5123,7 @@
       <c r="M33" s="14"/>
       <c r="N33" s="14"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f>IF(NOT(ISBLANK(C34)),Cover!$C$11,"")</f>
         <v/>
@@ -5135,7 +5138,7 @@
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f>IF(NOT(ISBLANK(C35)),Cover!$C$11,"")</f>
         <v/>
@@ -5150,31 +5153,31 @@
       <c r="M35" s="14"/>
       <c r="N35" s="14"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f>IF(NOT(ISBLANK(C36)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f>IF(NOT(ISBLANK(C37)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f>IF(NOT(ISBLANK(C38)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f>IF(NOT(ISBLANK(C39)),Cover!$C$11,"")</f>
         <v/>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f>IF(NOT(ISBLANK(C40)),Cover!$C$11,"")</f>
         <v/>

</xml_diff>